<commit_message>
Synchronize local repo, just notes
</commit_message>
<xml_diff>
--- a/animation-bulk-validation/IWP6_bulkValidate_Trello_2019Sep12.xlsx
+++ b/animation-bulk-validation/IWP6_bulkValidate_Trello_2019Sep12.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brockman/ncssm/git/iwphys/animation-bulk-validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{5197A9CB-8E7C-3843-95D6-B41FCFAA17E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB115A6B-3F14-7340-B856-765A474E523D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4460" yWindow="-21140" windowWidth="38400" windowHeight="21140"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2019Sep12_bulkValidate_Clean" sheetId="1" r:id="rId1"/>
@@ -2586,7 +2586,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -3139,7 +3139,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -3167,36 +3167,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3509,13 +3479,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P227"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="192" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A166" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="143" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="H39" sqref="H39"/>
+      <selection pane="bottomLeft" activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3588,7 +3558,7 @@
         <v>12</v>
       </c>
       <c r="B2" s="2" t="str">
-        <f>HYPERLINK(P2)</f>
+        <f t="shared" ref="B2:B65" si="0">HYPERLINK(P2)</f>
         <v>https://iwp6.iwphys.org/animation/ftemo/cp-mfield-02.iwp</v>
       </c>
       <c r="D2" t="s">
@@ -3607,7 +3577,7 @@
         <v>1620</v>
       </c>
       <c r="I2">
-        <f>H2/G2</f>
+        <f t="shared" ref="I2:I10" si="1">H2/G2</f>
         <v>1.9424460431654675</v>
       </c>
       <c r="J2" t="b">
@@ -3637,7 +3607,7 @@
         <v>12</v>
       </c>
       <c r="B3" s="2" t="str">
-        <f>HYPERLINK(P3)</f>
+        <f t="shared" si="0"/>
         <v>https://iwp6.iwphys.org/animation/ftemo/em-ratio-1b.iwp</v>
       </c>
       <c r="D3" t="s">
@@ -3656,7 +3626,7 @@
         <v>798</v>
       </c>
       <c r="I3">
-        <f>H3/G3</f>
+        <f t="shared" si="1"/>
         <v>3.99</v>
       </c>
       <c r="J3" t="b">
@@ -3686,7 +3656,7 @@
         <v>12</v>
       </c>
       <c r="B4" s="2" t="str">
-        <f>HYPERLINK(P4)</f>
+        <f t="shared" si="0"/>
         <v>https://iwp6.iwphys.org/animation/ftemo/em-ratio-1c.iwp</v>
       </c>
       <c r="D4" t="s">
@@ -3705,7 +3675,7 @@
         <v>305</v>
       </c>
       <c r="I4">
-        <f>H4/G4</f>
+        <f t="shared" si="1"/>
         <v>1.6223404255319149</v>
       </c>
       <c r="J4" t="b">
@@ -3735,7 +3705,7 @@
         <v>12</v>
       </c>
       <c r="B5" s="2" t="str">
-        <f>HYPERLINK(P5)</f>
+        <f t="shared" si="0"/>
         <v>https://iwp6.iwphys.org/animation/ftemo/em-ratio-1d.iwp</v>
       </c>
       <c r="D5" t="s">
@@ -3754,7 +3724,7 @@
         <v>1120</v>
       </c>
       <c r="I5">
-        <f>H5/G5</f>
+        <f t="shared" si="1"/>
         <v>5.6</v>
       </c>
       <c r="J5" t="b">
@@ -3784,7 +3754,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="2" t="str">
-        <f>HYPERLINK(P6)</f>
+        <f t="shared" si="0"/>
         <v>https://iwp6.iwphys.org/animation/ftemo/em-ratio-2d.iwp</v>
       </c>
       <c r="D6" t="s">
@@ -3803,7 +3773,7 @@
         <v>2836</v>
       </c>
       <c r="I6">
-        <f>H6/G6</f>
+        <f t="shared" si="1"/>
         <v>14.109452736318408</v>
       </c>
       <c r="J6" t="b">
@@ -3833,7 +3803,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="2" t="str">
-        <f>HYPERLINK(P7)</f>
+        <f t="shared" si="0"/>
         <v>https://iwp6.iwphys.org/animation/ftemo/lenzlaw-01.iwp</v>
       </c>
       <c r="D7" t="s">
@@ -3852,7 +3822,7 @@
         <v>35</v>
       </c>
       <c r="I7">
-        <f>H7/G7</f>
+        <f t="shared" si="1"/>
         <v>1.1290322580645162</v>
       </c>
       <c r="J7" t="b">
@@ -3882,7 +3852,7 @@
         <v>12</v>
       </c>
       <c r="B8" s="2" t="str">
-        <f>HYPERLINK(P8)</f>
+        <f t="shared" si="0"/>
         <v>https://iwp6.iwphys.org/animation/ftemo/lenzlaw-02b.iwp</v>
       </c>
       <c r="D8" t="s">
@@ -3901,7 +3871,7 @@
         <v>3</v>
       </c>
       <c r="I8">
-        <f>H8/G8</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="J8" t="b">
@@ -3931,7 +3901,7 @@
         <v>12</v>
       </c>
       <c r="B9" s="2" t="str">
-        <f>HYPERLINK(P9)</f>
+        <f t="shared" si="0"/>
         <v>https://iwp6.iwphys.org/animation/ftemo/mass-spec.iwp</v>
       </c>
       <c r="D9" t="s">
@@ -3950,7 +3920,7 @@
         <v>115</v>
       </c>
       <c r="I9">
-        <f>H9/G9</f>
+        <f t="shared" si="1"/>
         <v>1.7692307692307692</v>
       </c>
       <c r="J9" t="b">
@@ -3980,7 +3950,7 @@
         <v>12</v>
       </c>
       <c r="B10" s="2" t="str">
-        <f>HYPERLINK(P10)</f>
+        <f t="shared" si="0"/>
         <v>https://iwp6.iwphys.org/animation/ftemo/rainbow-01.iwp</v>
       </c>
       <c r="D10" t="s">
@@ -3999,7 +3969,7 @@
         <v>4</v>
       </c>
       <c r="I10">
-        <f>H10/G10</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="J10" t="b">
@@ -4029,7 +3999,7 @@
         <v>12</v>
       </c>
       <c r="B11" s="2" t="str">
-        <f>HYPERLINK(P11)</f>
+        <f t="shared" si="0"/>
         <v>https://iwp6.iwphys.org/animation/ftemo/ray-refraction-3i.iwp</v>
       </c>
       <c r="D11" t="s">
@@ -4077,7 +4047,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="2" t="str">
-        <f>HYPERLINK(P12)</f>
+        <f t="shared" si="0"/>
         <v>https://iwp6.iwphys.org/animation/ftemo/refracted-waves-5.iwp</v>
       </c>
       <c r="D12" t="s">
@@ -4096,7 +4066,7 @@
         <v>12</v>
       </c>
       <c r="I12">
-        <f>H12/G12</f>
+        <f t="shared" ref="I12:I20" si="2">H12/G12</f>
         <v>12</v>
       </c>
       <c r="J12" t="b">
@@ -4126,7 +4096,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="str">
-        <f>HYPERLINK(P13)</f>
+        <f t="shared" si="0"/>
         <v>https://iwp6.iwphys.org/animation/ftemo/refracted-waves-6b.iwp</v>
       </c>
       <c r="D13" t="s">
@@ -4145,7 +4115,7 @@
         <v>38</v>
       </c>
       <c r="I13">
-        <f>H13/G13</f>
+        <f t="shared" si="2"/>
         <v>38</v>
       </c>
       <c r="J13" t="b">
@@ -4175,7 +4145,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="2" t="str">
-        <f>HYPERLINK(P14)</f>
+        <f t="shared" si="0"/>
         <v>https://iwp6.iwphys.org/animation/iwp-2015/em-ratio-2f.iwp</v>
       </c>
       <c r="D14" t="s">
@@ -4194,7 +4164,7 @@
         <v>2836</v>
       </c>
       <c r="I14">
-        <f>H14/G14</f>
+        <f t="shared" si="2"/>
         <v>14.109452736318408</v>
       </c>
       <c r="J14" t="b">
@@ -4224,7 +4194,7 @@
         <v>12</v>
       </c>
       <c r="B15" s="2" t="str">
-        <f>HYPERLINK(P15)</f>
+        <f t="shared" si="0"/>
         <v>https://iwp6.iwphys.org/animation/iwp-2015/spring-motion-5.iwp</v>
       </c>
       <c r="D15" t="s">
@@ -4243,7 +4213,7 @@
         <v>9</v>
       </c>
       <c r="I15">
-        <f>H15/G15</f>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="J15" t="b">
@@ -4273,7 +4243,7 @@
         <v>12</v>
       </c>
       <c r="B16" s="2" t="str">
-        <f>HYPERLINK(P16)</f>
+        <f t="shared" si="0"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Charged Particle Motion/cp-efield-02.iwp</v>
       </c>
       <c r="D16" t="s">
@@ -4292,7 +4262,7 @@
         <v>4</v>
       </c>
       <c r="I16">
-        <f>H16/G16</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="J16" t="b">
@@ -4322,7 +4292,7 @@
         <v>12</v>
       </c>
       <c r="B17" s="2" t="str">
-        <f>HYPERLINK(P17)</f>
+        <f t="shared" si="0"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Charged Particle Motion/cp-efield.iwp</v>
       </c>
       <c r="D17" t="s">
@@ -4341,7 +4311,7 @@
         <v>4</v>
       </c>
       <c r="I17">
-        <f>H17/G17</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="J17" t="b">
@@ -4371,7 +4341,7 @@
         <v>12</v>
       </c>
       <c r="B18" s="2" t="str">
-        <f>HYPERLINK(P18)</f>
+        <f t="shared" si="0"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Charged Particle Motion/cp-mfield-02.iwp</v>
       </c>
       <c r="D18" t="s">
@@ -4390,7 +4360,7 @@
         <v>1620</v>
       </c>
       <c r="I18">
-        <f>H18/G18</f>
+        <f t="shared" si="2"/>
         <v>1.9424460431654675</v>
       </c>
       <c r="J18" t="b">
@@ -4420,7 +4390,7 @@
         <v>12</v>
       </c>
       <c r="B19" s="2" t="str">
-        <f>HYPERLINK(P19)</f>
+        <f t="shared" si="0"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Charged Particle Motion/cp-mfield.iwp</v>
       </c>
       <c r="D19" t="s">
@@ -4439,7 +4409,7 @@
         <v>1620</v>
       </c>
       <c r="I19">
-        <f>H19/G19</f>
+        <f t="shared" si="2"/>
         <v>1.9424460431654675</v>
       </c>
       <c r="J19" t="b">
@@ -4469,7 +4439,7 @@
         <v>12</v>
       </c>
       <c r="B20" s="2" t="str">
-        <f>HYPERLINK(P20)</f>
+        <f t="shared" si="0"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Charged Particle Motion/cp-template.iwp</v>
       </c>
       <c r="D20" t="s">
@@ -4488,7 +4458,7 @@
         <v>1833</v>
       </c>
       <c r="I20">
-        <f>H20/G20</f>
+        <f t="shared" si="2"/>
         <v>1.870408163265306</v>
       </c>
       <c r="J20" t="b">
@@ -4518,7 +4488,7 @@
         <v>12</v>
       </c>
       <c r="B21" s="2" t="str">
-        <f>HYPERLINK(P21)</f>
+        <f t="shared" si="0"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Charged Particle Motion/cp-unknown-1.iwp</v>
       </c>
       <c r="D21" t="s">
@@ -4566,7 +4536,7 @@
         <v>12</v>
       </c>
       <c r="B22" s="2" t="str">
-        <f>HYPERLINK(P22)</f>
+        <f t="shared" si="0"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Charged Particle Motion/cpchall01.iwp</v>
       </c>
       <c r="D22" t="s">
@@ -4585,7 +4555,7 @@
         <v>805</v>
       </c>
       <c r="I22">
-        <f>H22/G22</f>
+        <f t="shared" ref="I22:I29" si="3">H22/G22</f>
         <v>1</v>
       </c>
       <c r="J22" t="b">
@@ -4615,7 +4585,7 @@
         <v>12</v>
       </c>
       <c r="B23" s="2" t="str">
-        <f>HYPERLINK(P23)</f>
+        <f t="shared" si="0"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Charged Particle Motion/cpchall02.iwp</v>
       </c>
       <c r="D23" t="s">
@@ -4634,7 +4604,7 @@
         <v>847</v>
       </c>
       <c r="I23">
-        <f>H23/G23</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J23" t="b">
@@ -4664,7 +4634,7 @@
         <v>12</v>
       </c>
       <c r="B24" s="2" t="str">
-        <f>HYPERLINK(P24)</f>
+        <f t="shared" si="0"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Charged Particle Motion/cpchall03.iwp</v>
       </c>
       <c r="D24" t="s">
@@ -4683,7 +4653,7 @@
         <v>847</v>
       </c>
       <c r="I24">
-        <f>H24/G24</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J24" t="b">
@@ -4713,7 +4683,7 @@
         <v>12</v>
       </c>
       <c r="B25" s="2" t="str">
-        <f>HYPERLINK(P25)</f>
+        <f t="shared" si="0"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Charged Particle Motion/cpchall04.iwp</v>
       </c>
       <c r="D25" t="s">
@@ -4732,7 +4702,7 @@
         <v>805</v>
       </c>
       <c r="I25">
-        <f>H25/G25</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J25" t="b">
@@ -4762,7 +4732,7 @@
         <v>12</v>
       </c>
       <c r="B26" s="2" t="str">
-        <f>HYPERLINK(P26)</f>
+        <f t="shared" si="0"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Charged Particle Motion/em-ratio-1.iwp</v>
       </c>
       <c r="D26" t="s">
@@ -4781,7 +4751,7 @@
         <v>1478</v>
       </c>
       <c r="I26">
-        <f>H26/G26</f>
+        <f t="shared" si="3"/>
         <v>7.3532338308457712</v>
       </c>
       <c r="J26" t="b">
@@ -4811,7 +4781,7 @@
         <v>12</v>
       </c>
       <c r="B27" s="2" t="str">
-        <f>HYPERLINK(P27)</f>
+        <f t="shared" si="0"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Charged Particle Motion/em-ratio-1b.iwp</v>
       </c>
       <c r="D27" t="s">
@@ -4830,7 +4800,7 @@
         <v>798</v>
       </c>
       <c r="I27">
-        <f>H27/G27</f>
+        <f t="shared" si="3"/>
         <v>3.99</v>
       </c>
       <c r="J27" t="b">
@@ -4860,7 +4830,7 @@
         <v>12</v>
       </c>
       <c r="B28" s="2" t="str">
-        <f>HYPERLINK(P28)</f>
+        <f t="shared" si="0"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Charged Particle Motion/em-ratio-1c.iwp</v>
       </c>
       <c r="D28" t="s">
@@ -4879,7 +4849,7 @@
         <v>305</v>
       </c>
       <c r="I28">
-        <f>H28/G28</f>
+        <f t="shared" si="3"/>
         <v>1.6223404255319149</v>
       </c>
       <c r="J28" t="b">
@@ -4909,7 +4879,7 @@
         <v>12</v>
       </c>
       <c r="B29" s="2" t="str">
-        <f>HYPERLINK(P29)</f>
+        <f t="shared" si="0"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Charged Particle Motion/em-ratio-1d.iwp</v>
       </c>
       <c r="D29" t="s">
@@ -4928,7 +4898,7 @@
         <v>1120</v>
       </c>
       <c r="I29">
-        <f>H29/G29</f>
+        <f t="shared" si="3"/>
         <v>5.6</v>
       </c>
       <c r="J29" t="b">
@@ -4958,7 +4928,7 @@
         <v>12</v>
       </c>
       <c r="B30" s="2" t="str">
-        <f>HYPERLINK(P30)</f>
+        <f t="shared" si="0"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Charged Particle Motion/em-ratio-2.iwp</v>
       </c>
       <c r="D30" t="s">
@@ -5006,7 +4976,7 @@
         <v>12</v>
       </c>
       <c r="B31" s="2" t="str">
-        <f>HYPERLINK(P31)</f>
+        <f t="shared" si="0"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Charged Particle Motion/em-ratio-2b.iwp</v>
       </c>
       <c r="D31" t="s">
@@ -5025,7 +4995,7 @@
         <v>3784</v>
       </c>
       <c r="I31">
-        <f>H31/G31</f>
+        <f t="shared" ref="I31:I39" si="4">H31/G31</f>
         <v>18.82587064676617</v>
       </c>
       <c r="J31" t="b">
@@ -5055,7 +5025,7 @@
         <v>12</v>
       </c>
       <c r="B32" s="2" t="str">
-        <f>HYPERLINK(P32)</f>
+        <f t="shared" si="0"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Charged Particle Motion/em-ratio-2d.iwp</v>
       </c>
       <c r="D32" t="s">
@@ -5074,7 +5044,7 @@
         <v>2836</v>
       </c>
       <c r="I32">
-        <f>H32/G32</f>
+        <f t="shared" si="4"/>
         <v>14.109452736318408</v>
       </c>
       <c r="J32" t="b">
@@ -5104,7 +5074,7 @@
         <v>12</v>
       </c>
       <c r="B33" s="2" t="str">
-        <f>HYPERLINK(P33)</f>
+        <f t="shared" si="0"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Charged Particle Motion/pitch1-para.iwp</v>
       </c>
       <c r="D33" t="s">
@@ -5123,7 +5093,7 @@
         <v>18663</v>
       </c>
       <c r="I33">
-        <f>H33/G33</f>
+        <f t="shared" si="4"/>
         <v>18.663</v>
       </c>
       <c r="J33" t="b">
@@ -5153,7 +5123,7 @@
         <v>12</v>
       </c>
       <c r="B34" s="2" t="str">
-        <f>HYPERLINK(P34)</f>
+        <f t="shared" si="0"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Charged Particle Motion/velocity-selector-02.iwp</v>
       </c>
       <c r="D34" t="s">
@@ -5172,7 +5142,7 @@
         <v>586</v>
       </c>
       <c r="I34">
-        <f>H34/G34</f>
+        <f t="shared" si="4"/>
         <v>1.9276315789473684</v>
       </c>
       <c r="J34" t="b">
@@ -5202,7 +5172,7 @@
         <v>12</v>
       </c>
       <c r="B35" s="2" t="str">
-        <f>HYPERLINK(P35)</f>
+        <f t="shared" si="0"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Charged Particle Motion/velocity-selector.iwp</v>
       </c>
       <c r="D35" t="s">
@@ -5221,7 +5191,7 @@
         <v>586</v>
       </c>
       <c r="I35">
-        <f>H35/G35</f>
+        <f t="shared" si="4"/>
         <v>1.9276315789473684</v>
       </c>
       <c r="J35" t="b">
@@ -5251,7 +5221,7 @@
         <v>12</v>
       </c>
       <c r="B36" s="2" t="str">
-        <f>HYPERLINK(P36)</f>
+        <f t="shared" si="0"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Electrostatics/coulombslaw01.iwp</v>
       </c>
       <c r="D36" t="s">
@@ -5270,7 +5240,7 @@
         <v>5</v>
       </c>
       <c r="I36">
-        <f>H36/G36</f>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="J36" t="b">
@@ -5300,7 +5270,7 @@
         <v>12</v>
       </c>
       <c r="B37" s="2" t="str">
-        <f>HYPERLINK(P37)</f>
+        <f t="shared" si="0"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Electrostatics/efield-plot-02.iwp</v>
       </c>
       <c r="D37" t="s">
@@ -5319,7 +5289,7 @@
         <v>4</v>
       </c>
       <c r="I37">
-        <f>H37/G37</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="J37" t="b">
@@ -5349,7 +5319,7 @@
         <v>12</v>
       </c>
       <c r="B38" s="2" t="str">
-        <f>HYPERLINK(P38)</f>
+        <f t="shared" si="0"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Electrostatics/efield-plot-02a.iwp</v>
       </c>
       <c r="D38" t="s">
@@ -5368,7 +5338,7 @@
         <v>2</v>
       </c>
       <c r="I38">
-        <f>H38/G38</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="J38" t="b">
@@ -5398,7 +5368,7 @@
         <v>12</v>
       </c>
       <c r="B39" s="2" t="str">
-        <f>HYPERLINK(P39)</f>
+        <f t="shared" si="0"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Forces/bppb6.iwp</v>
       </c>
       <c r="D39" t="s">
@@ -5417,7 +5387,7 @@
         <v>1</v>
       </c>
       <c r="I39">
-        <f>H39/G39</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J39" t="b">
@@ -5447,7 +5417,7 @@
         <v>12</v>
       </c>
       <c r="B40" s="2" t="str">
-        <f>HYPERLINK(P40)</f>
+        <f t="shared" si="0"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Forces/fallcompare-simulation.iwp</v>
       </c>
       <c r="D40" t="s">
@@ -5495,7 +5465,7 @@
         <v>12</v>
       </c>
       <c r="B41" s="2" t="str">
-        <f>HYPERLINK(P41)</f>
+        <f t="shared" si="0"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Forces/hookeslaw03.iwp</v>
       </c>
       <c r="D41" t="s">
@@ -5544,7 +5514,7 @@
         <v>12</v>
       </c>
       <c r="B42" s="2" t="str">
-        <f>HYPERLINK(P42)</f>
+        <f t="shared" si="0"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Forces/leaf.iwp</v>
       </c>
       <c r="D42" t="s">
@@ -5592,7 +5562,7 @@
         <v>12</v>
       </c>
       <c r="B43" s="2" t="str">
-        <f>HYPERLINK(P43)</f>
+        <f t="shared" si="0"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Forces/mass-bppb-3.iwp</v>
       </c>
       <c r="D43" t="s">
@@ -5611,7 +5581,7 @@
         <v>2</v>
       </c>
       <c r="I43">
-        <f>H43/G43</f>
+        <f t="shared" ref="I43:I52" si="5">H43/G43</f>
         <v>2</v>
       </c>
       <c r="J43" t="b">
@@ -5641,7 +5611,7 @@
         <v>12</v>
       </c>
       <c r="B44" s="2" t="str">
-        <f>HYPERLINK(P44)</f>
+        <f t="shared" si="0"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Forces/projectile-drag-2.iwp</v>
       </c>
       <c r="D44" t="s">
@@ -5660,7 +5630,7 @@
         <v>6172</v>
       </c>
       <c r="I44">
-        <f>H44/G44</f>
+        <f t="shared" si="5"/>
         <v>6.1719999999999997</v>
       </c>
       <c r="J44" t="b">
@@ -5690,7 +5660,7 @@
         <v>12</v>
       </c>
       <c r="B45" s="2" t="str">
-        <f>HYPERLINK(P45)</f>
+        <f t="shared" si="0"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Forces/projectile-drag-lift-2.iwp</v>
       </c>
       <c r="D45" t="s">
@@ -5709,7 +5679,7 @@
         <v>997</v>
       </c>
       <c r="I45">
-        <f>H45/G45</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="J45" t="b">
@@ -5739,7 +5709,7 @@
         <v>12</v>
       </c>
       <c r="B46" s="2" t="str">
-        <f>HYPERLINK(P46)</f>
+        <f t="shared" si="0"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Gravitation/planetary-system-02.iwp</v>
       </c>
       <c r="D46" t="s">
@@ -5758,7 +5728,7 @@
         <v>8</v>
       </c>
       <c r="I46">
-        <f>H46/G46</f>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="J46" t="b">
@@ -5788,7 +5758,7 @@
         <v>12</v>
       </c>
       <c r="B47" s="2" t="str">
-        <f>HYPERLINK(P47)</f>
+        <f t="shared" si="0"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Gravitation/planetary-system-retrograde.iwp</v>
       </c>
       <c r="D47" t="s">
@@ -5807,7 +5777,7 @@
         <v>6</v>
       </c>
       <c r="I47">
-        <f>H47/G47</f>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="J47" t="b">
@@ -5837,7 +5807,7 @@
         <v>12</v>
       </c>
       <c r="B48" s="2" t="str">
-        <f>HYPERLINK(P48)</f>
+        <f t="shared" si="0"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Kinematics 1D/dvat-11.iwp</v>
       </c>
       <c r="D48" t="s">
@@ -5856,7 +5826,7 @@
         <v>2</v>
       </c>
       <c r="I48">
-        <f>H48/G48</f>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="J48" t="b">
@@ -5886,7 +5856,7 @@
         <v>12</v>
       </c>
       <c r="B49" s="2" t="str">
-        <f>HYPERLINK(P49)</f>
+        <f t="shared" si="0"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Kinematics 1D/haretortoise.iwp</v>
       </c>
       <c r="D49" t="s">
@@ -5905,7 +5875,7 @@
         <v>4</v>
       </c>
       <c r="I49">
-        <f>H49/G49</f>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="J49" t="b">
@@ -5935,7 +5905,7 @@
         <v>12</v>
       </c>
       <c r="B50" s="2" t="str">
-        <f>HYPERLINK(P50)</f>
+        <f t="shared" si="0"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Kinematics 1D/haretortoise2.iwp</v>
       </c>
       <c r="D50" t="s">
@@ -5954,7 +5924,7 @@
         <v>6</v>
       </c>
       <c r="I50">
-        <f>H50/G50</f>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="J50" t="b">
@@ -5984,7 +5954,7 @@
         <v>12</v>
       </c>
       <c r="B51" s="2" t="str">
-        <f>HYPERLINK(P51)</f>
+        <f t="shared" si="0"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Kinematics 1D/kingraph1.iwp</v>
       </c>
       <c r="D51" t="s">
@@ -6003,7 +5973,7 @@
         <v>2</v>
       </c>
       <c r="I51">
-        <f>H51/G51</f>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="J51" t="b">
@@ -6033,7 +6003,7 @@
         <v>12</v>
       </c>
       <c r="B52" s="2" t="str">
-        <f>HYPERLINK(P52)</f>
+        <f t="shared" si="0"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Kinematics 1D/kingraph2.iwp</v>
       </c>
       <c r="D52" t="s">
@@ -6052,7 +6022,7 @@
         <v>2</v>
       </c>
       <c r="I52">
-        <f>H52/G52</f>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="J52" t="b">
@@ -6082,7 +6052,7 @@
         <v>12</v>
       </c>
       <c r="B53" s="2" t="str">
-        <f>HYPERLINK(P53)</f>
+        <f t="shared" si="0"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Kinematics 1D/roadrage-bk.iwp</v>
       </c>
       <c r="D53" t="s">
@@ -6130,7 +6100,7 @@
         <v>12</v>
       </c>
       <c r="B54" s="2" t="str">
-        <f>HYPERLINK(P54)</f>
+        <f t="shared" si="0"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Kinematics 1D/velocity01.iwp</v>
       </c>
       <c r="D54" t="s">
@@ -6179,7 +6149,7 @@
         <v>12</v>
       </c>
       <c r="B55" s="2" t="str">
-        <f>HYPERLINK(P55)</f>
+        <f t="shared" si="0"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Kinematics 1D/velocity02.iwp</v>
       </c>
       <c r="D55" t="s">
@@ -6228,7 +6198,7 @@
         <v>12</v>
       </c>
       <c r="B56" s="2" t="str">
-        <f>HYPERLINK(P56)</f>
+        <f t="shared" si="0"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Kinematics 1D/velocity02b.iwp</v>
       </c>
       <c r="D56" t="s">
@@ -6277,7 +6247,7 @@
         <v>12</v>
       </c>
       <c r="B57" s="2" t="str">
-        <f>HYPERLINK(P57)</f>
+        <f t="shared" si="0"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Kinematics 1D/velocity03.iwp</v>
       </c>
       <c r="D57" t="s">
@@ -6326,7 +6296,7 @@
         <v>12</v>
       </c>
       <c r="B58" s="2" t="str">
-        <f>HYPERLINK(P58)</f>
+        <f t="shared" si="0"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Kinematics 1D/window01.iwp</v>
       </c>
       <c r="D58" t="s">
@@ -6375,7 +6345,7 @@
         <v>12</v>
       </c>
       <c r="B59" s="2" t="str">
-        <f>HYPERLINK(P59)</f>
+        <f t="shared" si="0"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Kinematics 2D/clock-02.iwp</v>
       </c>
       <c r="D59" t="s">
@@ -6423,7 +6393,7 @@
         <v>12</v>
       </c>
       <c r="B60" s="2" t="str">
-        <f>HYPERLINK(P60)</f>
+        <f t="shared" si="0"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Kinematics 2D/dartgun3.iwp</v>
       </c>
       <c r="D60" t="s">
@@ -6472,7 +6442,7 @@
         <v>12</v>
       </c>
       <c r="B61" s="2" t="str">
-        <f>HYPERLINK(P61)</f>
+        <f t="shared" si="0"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Kinematics 2D/globalcrossing-bk.iwp</v>
       </c>
       <c r="D61" t="s">
@@ -6521,7 +6491,7 @@
         <v>12</v>
       </c>
       <c r="B62" s="2" t="str">
-        <f>HYPERLINK(P62)</f>
+        <f t="shared" si="0"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Kinematics 2D/mgr1-2.iwp</v>
       </c>
       <c r="D62" t="s">
@@ -6570,7 +6540,7 @@
         <v>12</v>
       </c>
       <c r="B63" s="2" t="str">
-        <f>HYPERLINK(P63)</f>
+        <f t="shared" si="0"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Kinematics 2D/pursuit-template.iwp</v>
       </c>
       <c r="D63" t="s">
@@ -6619,7 +6589,7 @@
         <v>12</v>
       </c>
       <c r="B64" s="2" t="str">
-        <f>HYPERLINK(P64)</f>
+        <f t="shared" si="0"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Kinematics 2D/race-template-2.iwp</v>
       </c>
       <c r="D64" t="s">
@@ -6668,7 +6638,7 @@
         <v>12</v>
       </c>
       <c r="B65" s="2" t="str">
-        <f>HYPERLINK(P65)</f>
+        <f t="shared" si="0"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Kinematics 2D/vector01.iwp</v>
       </c>
       <c r="D65" t="s">
@@ -6716,7 +6686,7 @@
         <v>12</v>
       </c>
       <c r="B66" s="2" t="str">
-        <f>HYPERLINK(P66)</f>
+        <f t="shared" ref="B66:B129" si="6">HYPERLINK(P66)</f>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Magnetism/helmholtz-3.iwp</v>
       </c>
       <c r="D66" t="s">
@@ -6735,7 +6705,7 @@
         <v>8</v>
       </c>
       <c r="I66">
-        <f>H66/G66</f>
+        <f t="shared" ref="I66:I106" si="7">H66/G66</f>
         <v>8</v>
       </c>
       <c r="J66" t="b">
@@ -6765,7 +6735,7 @@
         <v>12</v>
       </c>
       <c r="B67" s="2" t="str">
-        <f>HYPERLINK(P67)</f>
+        <f t="shared" si="6"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Momentum, Collisions, KE/collision-elastic-2.iwp</v>
       </c>
       <c r="D67" t="s">
@@ -6784,7 +6754,7 @@
         <v>2</v>
       </c>
       <c r="I67">
-        <f>H67/G67</f>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="J67" t="b">
@@ -6814,7 +6784,7 @@
         <v>12</v>
       </c>
       <c r="B68" s="2" t="str">
-        <f>HYPERLINK(P68)</f>
+        <f t="shared" si="6"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Momentum, Collisions, KE/collision-elastic-3.iwp</v>
       </c>
       <c r="D68" t="s">
@@ -6833,7 +6803,7 @@
         <v>3</v>
       </c>
       <c r="I68">
-        <f>H68/G68</f>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="J68" t="b">
@@ -6863,7 +6833,7 @@
         <v>12</v>
       </c>
       <c r="B69" s="2" t="str">
-        <f>HYPERLINK(P69)</f>
+        <f t="shared" si="6"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Momentum, Collisions, KE/collision-elastic-4.iwp</v>
       </c>
       <c r="D69" t="s">
@@ -6882,7 +6852,7 @@
         <v>2</v>
       </c>
       <c r="I69">
-        <f>H69/G69</f>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="J69" t="b">
@@ -6912,7 +6882,7 @@
         <v>12</v>
       </c>
       <c r="B70" s="2" t="str">
-        <f>HYPERLINK(P70)</f>
+        <f t="shared" si="6"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Momentum, Collisions, KE/collision-inelastic-01a.iwp</v>
       </c>
       <c r="D70" t="s">
@@ -6931,7 +6901,7 @@
         <v>1</v>
       </c>
       <c r="I70">
-        <f>H70/G70</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="J70" t="b">
@@ -6961,7 +6931,7 @@
         <v>12</v>
       </c>
       <c r="B71" s="2" t="str">
-        <f>HYPERLINK(P71)</f>
+        <f t="shared" si="6"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Momentum, Collisions, KE/collision-inelastic-01b.iwp</v>
       </c>
       <c r="D71" t="s">
@@ -6980,7 +6950,7 @@
         <v>1</v>
       </c>
       <c r="I71">
-        <f>H71/G71</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="J71" t="b">
@@ -7010,7 +6980,7 @@
         <v>12</v>
       </c>
       <c r="B72" s="2" t="str">
-        <f>HYPERLINK(P72)</f>
+        <f t="shared" si="6"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Momentum, Collisions, KE/collision-inelastic-02a.iwp</v>
       </c>
       <c r="D72" t="s">
@@ -7029,7 +6999,7 @@
         <v>1</v>
       </c>
       <c r="I72">
-        <f>H72/G72</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="J72" t="b">
@@ -7059,7 +7029,7 @@
         <v>12</v>
       </c>
       <c r="B73" s="2" t="str">
-        <f>HYPERLINK(P73)</f>
+        <f t="shared" si="6"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Momentum, Collisions, KE/collision-inelastic-02b.iwp</v>
       </c>
       <c r="D73" t="s">
@@ -7078,7 +7048,7 @@
         <v>1</v>
       </c>
       <c r="I73">
-        <f>H73/G73</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="J73" t="b">
@@ -7108,7 +7078,7 @@
         <v>12</v>
       </c>
       <c r="B74" s="2" t="str">
-        <f>HYPERLINK(P74)</f>
+        <f t="shared" si="6"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Momentum, Collisions, KE/collision-inelastic-03a.iwp</v>
       </c>
       <c r="D74" t="s">
@@ -7127,7 +7097,7 @@
         <v>2</v>
       </c>
       <c r="I74">
-        <f>H74/G74</f>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="J74" t="b">
@@ -7157,7 +7127,7 @@
         <v>12</v>
       </c>
       <c r="B75" s="2" t="str">
-        <f>HYPERLINK(P75)</f>
+        <f t="shared" si="6"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Momentum, Collisions, KE/collision-inelastic-03b.iwp</v>
       </c>
       <c r="D75" t="s">
@@ -7176,7 +7146,7 @@
         <v>2</v>
       </c>
       <c r="I75">
-        <f>H75/G75</f>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="J75" t="b">
@@ -7206,7 +7176,7 @@
         <v>12</v>
       </c>
       <c r="B76" s="2" t="str">
-        <f>HYPERLINK(P76)</f>
+        <f t="shared" si="6"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Momentum, Collisions, KE/collision-inelastic-04a.iwp</v>
       </c>
       <c r="D76" t="s">
@@ -7225,7 +7195,7 @@
         <v>2</v>
       </c>
       <c r="I76">
-        <f>H76/G76</f>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="J76" t="b">
@@ -7255,7 +7225,7 @@
         <v>12</v>
       </c>
       <c r="B77" s="2" t="str">
-        <f>HYPERLINK(P77)</f>
+        <f t="shared" si="6"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Momentum, Collisions, KE/collision-inelastic-04b.iwp</v>
       </c>
       <c r="D77" t="s">
@@ -7274,7 +7244,7 @@
         <v>2</v>
       </c>
       <c r="I77">
-        <f>H77/G77</f>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="J77" t="b">
@@ -7304,7 +7274,7 @@
         <v>12</v>
       </c>
       <c r="B78" s="2" t="str">
-        <f>HYPERLINK(P78)</f>
+        <f t="shared" si="6"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Momentum, Collisions, KE/collision-inelastic-05.iwp</v>
       </c>
       <c r="D78" t="s">
@@ -7323,7 +7293,7 @@
         <v>2</v>
       </c>
       <c r="I78">
-        <f>H78/G78</f>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="J78" t="b">
@@ -7353,7 +7323,7 @@
         <v>12</v>
       </c>
       <c r="B79" s="2" t="str">
-        <f>HYPERLINK(P79)</f>
+        <f t="shared" si="6"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Momentum, Collisions, KE/collision-inelastic-template.iwp</v>
       </c>
       <c r="D79" t="s">
@@ -7372,7 +7342,7 @@
         <v>1</v>
       </c>
       <c r="I79">
-        <f>H79/G79</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="J79" t="b">
@@ -7402,7 +7372,7 @@
         <v>12</v>
       </c>
       <c r="B80" s="2" t="str">
-        <f>HYPERLINK(P80)</f>
+        <f t="shared" si="6"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Momentum, Collisions, KE/collision-symmetric.iwp</v>
       </c>
       <c r="D80" t="s">
@@ -7421,7 +7391,7 @@
         <v>1</v>
       </c>
       <c r="I80">
-        <f>H80/G80</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="J80" t="b">
@@ -7451,7 +7421,7 @@
         <v>12</v>
       </c>
       <c r="B81" s="2" t="str">
-        <f>HYPERLINK(P81)</f>
+        <f t="shared" si="6"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Momentum, Collisions, KE/finalke-03.iwp</v>
       </c>
       <c r="D81" t="s">
@@ -7470,7 +7440,7 @@
         <v>12</v>
       </c>
       <c r="I81">
-        <f>H81/G81</f>
+        <f t="shared" si="7"/>
         <v>12</v>
       </c>
       <c r="J81" t="b">
@@ -7500,7 +7470,7 @@
         <v>12</v>
       </c>
       <c r="B82" s="2" t="str">
-        <f>HYPERLINK(P82)</f>
+        <f t="shared" si="6"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Optics, Geometric/least-time-6.iwp</v>
       </c>
       <c r="D82" t="s">
@@ -7519,7 +7489,7 @@
         <v>8</v>
       </c>
       <c r="I82">
-        <f>H82/G82</f>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
       <c r="J82" t="b">
@@ -7549,7 +7519,7 @@
         <v>12</v>
       </c>
       <c r="B83" s="2" t="str">
-        <f>HYPERLINK(P83)</f>
+        <f t="shared" si="6"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Optics, Geometric/refracted-waves-3.iwp</v>
       </c>
       <c r="D83" t="s">
@@ -7568,7 +7538,7 @@
         <v>12</v>
       </c>
       <c r="I83">
-        <f>H83/G83</f>
+        <f t="shared" si="7"/>
         <v>12</v>
       </c>
       <c r="J83" t="b">
@@ -7598,7 +7568,7 @@
         <v>12</v>
       </c>
       <c r="B84" s="2" t="str">
-        <f>HYPERLINK(P84)</f>
+        <f t="shared" si="6"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Optics, Geometric/refracted-waves-4.iwp</v>
       </c>
       <c r="D84" t="s">
@@ -7617,7 +7587,7 @@
         <v>12</v>
       </c>
       <c r="I84">
-        <f>H84/G84</f>
+        <f t="shared" si="7"/>
         <v>12</v>
       </c>
       <c r="J84" t="b">
@@ -7647,7 +7617,7 @@
         <v>12</v>
       </c>
       <c r="B85" s="2" t="str">
-        <f>HYPERLINK(P85)</f>
+        <f t="shared" si="6"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Optics, Geometric/refracted-waves-5.iwp</v>
       </c>
       <c r="D85" t="s">
@@ -7666,7 +7636,7 @@
         <v>12</v>
       </c>
       <c r="I85">
-        <f>H85/G85</f>
+        <f t="shared" si="7"/>
         <v>12</v>
       </c>
       <c r="J85" t="b">
@@ -7696,7 +7666,7 @@
         <v>12</v>
       </c>
       <c r="B86" s="2" t="str">
-        <f>HYPERLINK(P86)</f>
+        <f t="shared" si="6"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Optics, Physical/2-source-inter.iwp</v>
       </c>
       <c r="D86" t="s">
@@ -7715,7 +7685,7 @@
         <v>40</v>
       </c>
       <c r="I86">
-        <f>H86/G86</f>
+        <f t="shared" si="7"/>
         <v>40</v>
       </c>
       <c r="J86" t="b">
@@ -7745,7 +7715,7 @@
         <v>12</v>
       </c>
       <c r="B87" s="2" t="str">
-        <f>HYPERLINK(P87)</f>
+        <f t="shared" si="6"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Oscillations/damped-1.iwp</v>
       </c>
       <c r="D87" t="s">
@@ -7764,7 +7734,7 @@
         <v>4</v>
       </c>
       <c r="I87">
-        <f>H87/G87</f>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="J87" t="b">
@@ -7794,7 +7764,7 @@
         <v>12</v>
       </c>
       <c r="B88" s="2" t="str">
-        <f>HYPERLINK(P88)</f>
+        <f t="shared" si="6"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Oscillations/damped-SHM-template.iwp</v>
       </c>
       <c r="D88" t="s">
@@ -7813,7 +7783,7 @@
         <v>2</v>
       </c>
       <c r="I88">
-        <f>H88/G88</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="J88" t="b">
@@ -7843,7 +7813,7 @@
         <v>12</v>
       </c>
       <c r="B89" s="2" t="str">
-        <f>HYPERLINK(P89)</f>
+        <f t="shared" si="6"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Oscillations/lissajous-figures.iwp</v>
       </c>
       <c r="D89" t="s">
@@ -7862,7 +7832,7 @@
         <v>2</v>
       </c>
       <c r="I89">
-        <f>H89/G89</f>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="J89" t="b">
@@ -7892,7 +7862,7 @@
         <v>12</v>
       </c>
       <c r="B90" s="2" t="str">
-        <f>HYPERLINK(P90)</f>
+        <f t="shared" si="6"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Oscillations/pendulum01.iwp</v>
       </c>
       <c r="D90" t="s">
@@ -7911,7 +7881,7 @@
         <v>6421</v>
       </c>
       <c r="I90">
-        <f>H90/G90</f>
+        <f t="shared" si="7"/>
         <v>12.816367265469061</v>
       </c>
       <c r="J90" t="b">
@@ -7941,7 +7911,7 @@
         <v>12</v>
       </c>
       <c r="B91" s="2" t="str">
-        <f>HYPERLINK(P91)</f>
+        <f t="shared" si="6"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Oscillations/shm-01.iwp</v>
       </c>
       <c r="D91" t="s">
@@ -7960,7 +7930,7 @@
         <v>2</v>
       </c>
       <c r="I91">
-        <f>H91/G91</f>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="J91" t="b">
@@ -7990,7 +7960,7 @@
         <v>12</v>
       </c>
       <c r="B92" s="2" t="str">
-        <f>HYPERLINK(P92)</f>
+        <f t="shared" si="6"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Oscillations/shm-02.iwp</v>
       </c>
       <c r="D92" t="s">
@@ -8009,7 +7979,7 @@
         <v>2</v>
       </c>
       <c r="I92">
-        <f>H92/G92</f>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="J92" t="b">
@@ -8039,7 +8009,7 @@
         <v>12</v>
       </c>
       <c r="B93" s="2" t="str">
-        <f>HYPERLINK(P93)</f>
+        <f t="shared" si="6"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Oscillations/shm-compare-01.iwp</v>
       </c>
       <c r="D93" t="s">
@@ -8058,7 +8028,7 @@
         <v>2</v>
       </c>
       <c r="I93">
-        <f>H93/G93</f>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="J93" t="b">
@@ -8088,7 +8058,7 @@
         <v>12</v>
       </c>
       <c r="B94" s="2" t="str">
-        <f>HYPERLINK(P94)</f>
+        <f t="shared" si="6"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Oscillations/shm-compare-template.iwp</v>
       </c>
       <c r="D94" t="s">
@@ -8107,7 +8077,7 @@
         <v>4</v>
       </c>
       <c r="I94">
-        <f>H94/G94</f>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="J94" t="b">
@@ -8137,7 +8107,7 @@
         <v>12</v>
       </c>
       <c r="B95" s="2" t="str">
-        <f>HYPERLINK(P95)</f>
+        <f t="shared" si="6"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Oscillations/shm-graph-01.iwp</v>
       </c>
       <c r="D95" t="s">
@@ -8156,7 +8126,7 @@
         <v>4</v>
       </c>
       <c r="I95">
-        <f>H95/G95</f>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="J95" t="b">
@@ -8186,7 +8156,7 @@
         <v>12</v>
       </c>
       <c r="B96" s="2" t="str">
-        <f>HYPERLINK(P96)</f>
+        <f t="shared" si="6"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Oscillations/shm-graph-02.iwp</v>
       </c>
       <c r="D96" t="s">
@@ -8205,7 +8175,7 @@
         <v>2</v>
       </c>
       <c r="I96">
-        <f>H96/G96</f>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="J96" t="b">
@@ -8235,7 +8205,7 @@
         <v>12</v>
       </c>
       <c r="B97" s="2" t="str">
-        <f>HYPERLINK(P97)</f>
+        <f t="shared" si="6"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Oscillations/shm-phase-01.iwp</v>
       </c>
       <c r="D97" t="s">
@@ -8254,7 +8224,7 @@
         <v>4</v>
       </c>
       <c r="I97">
-        <f>H97/G97</f>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="J97" t="b">
@@ -8284,7 +8254,7 @@
         <v>12</v>
       </c>
       <c r="B98" s="2" t="str">
-        <f>HYPERLINK(P98)</f>
+        <f t="shared" si="6"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Oscillations/shm-phase-02.iwp</v>
       </c>
       <c r="D98" t="s">
@@ -8303,7 +8273,7 @@
         <v>4</v>
       </c>
       <c r="I98">
-        <f>H98/G98</f>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="J98" t="b">
@@ -8333,7 +8303,7 @@
         <v>12</v>
       </c>
       <c r="B99" s="2" t="str">
-        <f>HYPERLINK(P99)</f>
+        <f t="shared" si="6"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Oscillations/shm-phase-03.iwp</v>
       </c>
       <c r="D99" t="s">
@@ -8352,7 +8322,7 @@
         <v>4</v>
       </c>
       <c r="I99">
-        <f>H99/G99</f>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="J99" t="b">
@@ -8382,7 +8352,7 @@
         <v>12</v>
       </c>
       <c r="B100" s="2" t="str">
-        <f>HYPERLINK(P100)</f>
+        <f t="shared" si="6"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Oscillations/shm-synchronize-02.iwp</v>
       </c>
       <c r="D100" t="s">
@@ -8401,7 +8371,7 @@
         <v>2</v>
       </c>
       <c r="I100">
-        <f>H100/G100</f>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="J100" t="b">
@@ -8431,7 +8401,7 @@
         <v>12</v>
       </c>
       <c r="B101" s="2" t="str">
-        <f>HYPERLINK(P101)</f>
+        <f t="shared" si="6"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Oscillations/shm-synchronize.iwp</v>
       </c>
       <c r="D101" t="s">
@@ -8450,7 +8420,7 @@
         <v>2</v>
       </c>
       <c r="I101">
-        <f>H101/G101</f>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="J101" t="b">
@@ -8480,7 +8450,7 @@
         <v>12</v>
       </c>
       <c r="B102" s="2" t="str">
-        <f>HYPERLINK(P102)</f>
+        <f t="shared" si="6"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Oscillations/shm-xva-plot.iwp</v>
       </c>
       <c r="D102" t="s">
@@ -8499,7 +8469,7 @@
         <v>7</v>
       </c>
       <c r="I102">
-        <f>H102/G102</f>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
       <c r="J102" t="b">
@@ -8529,7 +8499,7 @@
         <v>12</v>
       </c>
       <c r="B103" s="2" t="str">
-        <f>HYPERLINK(P103)</f>
+        <f t="shared" si="6"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Oscillations/spring-motion.iwp</v>
       </c>
       <c r="D103" t="s">
@@ -8548,7 +8518,7 @@
         <v>7</v>
       </c>
       <c r="I103">
-        <f>H103/G103</f>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
       <c r="J103" t="b">
@@ -8578,7 +8548,7 @@
         <v>12</v>
       </c>
       <c r="B104" s="2" t="str">
-        <f>HYPERLINK(P104)</f>
+        <f t="shared" si="6"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Oscillations/vertical-spring-01.iwp</v>
       </c>
       <c r="D104" t="s">
@@ -8597,7 +8567,7 @@
         <v>5</v>
       </c>
       <c r="I104">
-        <f>H104/G104</f>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="J104" t="b">
@@ -8627,7 +8597,7 @@
         <v>12</v>
       </c>
       <c r="B105" s="2" t="str">
-        <f>HYPERLINK(P105)</f>
+        <f t="shared" si="6"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/TEST Developer Test/TEST_attachedVectors.iwp</v>
       </c>
       <c r="D105" t="s">
@@ -8646,7 +8616,7 @@
         <v>4</v>
       </c>
       <c r="I105">
-        <f>H105/G105</f>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="J105" t="b">
@@ -8676,7 +8646,7 @@
         <v>12</v>
       </c>
       <c r="B106" s="2" t="str">
-        <f>HYPERLINK(P106)</f>
+        <f t="shared" si="6"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/TEST Developer Test/TEST_attachedXAccelZero.iwp</v>
       </c>
       <c r="D106" t="s">
@@ -8695,7 +8665,7 @@
         <v>1</v>
       </c>
       <c r="I106">
-        <f>H106/G106</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="J106" t="b">
@@ -8725,7 +8695,7 @@
         <v>12</v>
       </c>
       <c r="B107" s="2" t="str">
-        <f>HYPERLINK(P107)</f>
+        <f t="shared" si="6"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/TEST Developer Test/TEST_euler.iwp</v>
       </c>
       <c r="D107" t="s">
@@ -8773,7 +8743,7 @@
         <v>12</v>
       </c>
       <c r="B108" s="2" t="str">
-        <f>HYPERLINK(P108)</f>
+        <f t="shared" si="6"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/TEST Developer Test/TEST_eulerCrossPath.iwp</v>
       </c>
       <c r="D108" t="s">
@@ -8822,7 +8792,7 @@
         <v>12</v>
       </c>
       <c r="B109" s="2" t="str">
-        <f>HYPERLINK(P109)</f>
+        <f t="shared" si="6"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/TEST Developer Test/TEST_FloatingText.iwp</v>
       </c>
       <c r="D109" t="s">
@@ -8871,7 +8841,7 @@
         <v>12</v>
       </c>
       <c r="B110" s="2" t="str">
-        <f>HYPERLINK(P110)</f>
+        <f t="shared" si="6"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/TEST Developer Test/TEST_graph.iwp</v>
       </c>
       <c r="D110" t="s">
@@ -8920,7 +8890,7 @@
         <v>12</v>
       </c>
       <c r="B111" s="2" t="str">
-        <f>HYPERLINK(P111)</f>
+        <f t="shared" si="6"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/TEST Developer Test/TEST_hiddenInputs.iwp</v>
       </c>
       <c r="D111" t="s">
@@ -8968,7 +8938,7 @@
         <v>12</v>
       </c>
       <c r="B112" s="2" t="str">
-        <f>HYPERLINK(P112)</f>
+        <f t="shared" si="6"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/TEST Developer Test/TEST_inputoutput.iwp</v>
       </c>
       <c r="D112" t="s">
@@ -9016,7 +8986,7 @@
         <v>12</v>
       </c>
       <c r="B113" s="2" t="str">
-        <f>HYPERLINK(P113)</f>
+        <f t="shared" si="6"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/TEST Developer Test/TEST_inputs.iwp</v>
       </c>
       <c r="D113" t="s">
@@ -9065,7 +9035,7 @@
         <v>12</v>
       </c>
       <c r="B114" s="2" t="str">
-        <f>HYPERLINK(P114)</f>
+        <f t="shared" si="6"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/TEST Developer Test/TEST_mathOps.iwp</v>
       </c>
       <c r="D114" t="s">
@@ -9113,7 +9083,7 @@
         <v>12</v>
       </c>
       <c r="B115" s="2" t="str">
-        <f>HYPERLINK(P115)</f>
+        <f t="shared" si="6"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/TEST Developer Test/TEST_random.iwp</v>
       </c>
       <c r="D115" t="s">
@@ -9162,7 +9132,7 @@
         <v>12</v>
       </c>
       <c r="B116" s="2" t="str">
-        <f>HYPERLINK(P116)</f>
+        <f t="shared" si="6"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/TEST Developer Test/TEST_self.iwp</v>
       </c>
       <c r="D116" t="s">
@@ -9211,7 +9181,7 @@
         <v>12</v>
       </c>
       <c r="B117" s="2" t="str">
-        <f>HYPERLINK(P117)</f>
+        <f t="shared" si="6"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/TEST Developer Test/TEST_solidReadsOutput.iwp</v>
       </c>
       <c r="D117" t="s">
@@ -9260,7 +9230,7 @@
         <v>12</v>
       </c>
       <c r="B118" s="2" t="str">
-        <f>HYPERLINK(P118)</f>
+        <f t="shared" si="6"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/TEST Developer Test/TEST_time.iwp</v>
       </c>
       <c r="D118" t="s">
@@ -9308,7 +9278,7 @@
         <v>12</v>
       </c>
       <c r="B119" s="2" t="str">
-        <f>HYPERLINK(P119)</f>
+        <f t="shared" si="6"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/TEST Developer Test/TEST_trails.iwp</v>
       </c>
       <c r="D119" t="s">
@@ -9357,7 +9327,7 @@
         <v>12</v>
       </c>
       <c r="B120" s="2" t="str">
-        <f>HYPERLINK(P120)</f>
+        <f t="shared" si="6"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/TEST Developer Test/TEST_vectorShape.iwp</v>
       </c>
       <c r="D120" t="s">
@@ -9405,7 +9375,7 @@
         <v>12</v>
       </c>
       <c r="B121" s="2" t="str">
-        <f>HYPERLINK(P121)</f>
+        <f t="shared" si="6"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/TEST Developer Test/TEST_verySmall.iwp</v>
       </c>
       <c r="D121" t="s">
@@ -9424,7 +9394,7 @@
         <v>62</v>
       </c>
       <c r="I121">
-        <f>H121/G121</f>
+        <f t="shared" ref="I121:I145" si="8">H121/G121</f>
         <v>2</v>
       </c>
       <c r="J121" t="b">
@@ -9454,7 +9424,7 @@
         <v>12</v>
       </c>
       <c r="B122" s="2" t="str">
-        <f>HYPERLINK(P122)</f>
+        <f t="shared" si="6"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Waves and Sound/beats.iwp</v>
       </c>
       <c r="D122" t="s">
@@ -9473,7 +9443,7 @@
         <v>6</v>
       </c>
       <c r="I122">
-        <f>H122/G122</f>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
       <c r="J122" t="b">
@@ -9503,7 +9473,7 @@
         <v>12</v>
       </c>
       <c r="B123" s="2" t="str">
-        <f>HYPERLINK(P123)</f>
+        <f t="shared" si="6"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Waves and Sound/doppler4.iwp</v>
       </c>
       <c r="D123" t="s">
@@ -9522,7 +9492,7 @@
         <v>1</v>
       </c>
       <c r="I123">
-        <f>H123/G123</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="J123" t="b">
@@ -9552,7 +9522,7 @@
         <v>12</v>
       </c>
       <c r="B124" s="2" t="str">
-        <f>HYPERLINK(P124)</f>
+        <f t="shared" si="6"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Waves and Sound/doppler5.iwp</v>
       </c>
       <c r="D124" t="s">
@@ -9571,7 +9541,7 @@
         <v>1</v>
       </c>
       <c r="I124">
-        <f>H124/G124</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="J124" t="b">
@@ -9601,7 +9571,7 @@
         <v>12</v>
       </c>
       <c r="B125" s="2" t="str">
-        <f>HYPERLINK(P125)</f>
+        <f t="shared" si="6"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Waves and Sound/plucked-cord.iwp</v>
       </c>
       <c r="D125" t="s">
@@ -9620,7 +9590,7 @@
         <v>12</v>
       </c>
       <c r="I125">
-        <f>H125/G125</f>
+        <f t="shared" si="8"/>
         <v>12</v>
       </c>
       <c r="J125" t="b">
@@ -9650,7 +9620,7 @@
         <v>12</v>
       </c>
       <c r="B126" s="2" t="str">
-        <f>HYPERLINK(P126)</f>
+        <f t="shared" si="6"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Waves and Sound/trav-wave-3.iwp</v>
       </c>
       <c r="D126" t="s">
@@ -9669,7 +9639,7 @@
         <v>23</v>
       </c>
       <c r="I126">
-        <f>H126/G126</f>
+        <f t="shared" si="8"/>
         <v>23</v>
       </c>
       <c r="J126" t="b">
@@ -9699,7 +9669,7 @@
         <v>12</v>
       </c>
       <c r="B127" s="2" t="str">
-        <f>HYPERLINK(P127)</f>
+        <f t="shared" si="6"/>
         <v>https://iwp6.iwphys.org/animation/iwp-packaged/Waves and Sound/wavedraw.iwp</v>
       </c>
       <c r="D127" t="s">
@@ -9718,7 +9688,7 @@
         <v>4</v>
       </c>
       <c r="I127">
-        <f>H127/G127</f>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="J127" t="b">
@@ -9748,7 +9718,7 @@
         <v>12</v>
       </c>
       <c r="B128" s="2" t="str">
-        <f>HYPERLINK(P128)</f>
+        <f t="shared" si="6"/>
         <v>https://iwp6.iwphys.org/animation/summer-physics/040301.iwp</v>
       </c>
       <c r="D128" t="s">
@@ -9767,7 +9737,7 @@
         <v>2</v>
       </c>
       <c r="I128">
-        <f>H128/G128</f>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="J128" t="b">
@@ -9797,7 +9767,7 @@
         <v>12</v>
       </c>
       <c r="B129" s="2" t="str">
-        <f>HYPERLINK(P129)</f>
+        <f t="shared" si="6"/>
         <v>https://iwp6.iwphys.org/animation/summer-physics/040302.iwp</v>
       </c>
       <c r="D129" t="s">
@@ -9816,7 +9786,7 @@
         <v>1002</v>
       </c>
       <c r="I129">
-        <f>H129/G129</f>
+        <f t="shared" si="8"/>
         <v>1.002</v>
       </c>
       <c r="J129" t="b">
@@ -9846,7 +9816,7 @@
         <v>12</v>
       </c>
       <c r="B130" s="2" t="str">
-        <f>HYPERLINK(P130)</f>
+        <f t="shared" ref="B130:B193" si="9">HYPERLINK(P130)</f>
         <v>https://iwp6.iwphys.org/animation/summer-physics/040305.iwp</v>
       </c>
       <c r="D130" t="s">
@@ -9865,7 +9835,7 @@
         <v>1999</v>
       </c>
       <c r="I130">
-        <f>H130/G130</f>
+        <f t="shared" si="8"/>
         <v>2.0010010010010011</v>
       </c>
       <c r="J130" t="b">
@@ -9895,7 +9865,7 @@
         <v>12</v>
       </c>
       <c r="B131" s="2" t="str">
-        <f>HYPERLINK(P131)</f>
+        <f t="shared" si="9"/>
         <v>https://iwp6.iwphys.org/animation/summer-physics/atwoods-01.iwp</v>
       </c>
       <c r="D131" t="s">
@@ -9914,7 +9884,7 @@
         <v>4</v>
       </c>
       <c r="I131">
-        <f>H131/G131</f>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="J131" t="b">
@@ -9944,7 +9914,7 @@
         <v>12</v>
       </c>
       <c r="B132" s="2" t="str">
-        <f>HYPERLINK(P132)</f>
+        <f t="shared" si="9"/>
         <v>https://iwp6.iwphys.org/animation/summer-physics/auto-impulse-3.iwp</v>
       </c>
       <c r="D132" t="s">
@@ -9963,7 +9933,7 @@
         <v>55</v>
       </c>
       <c r="I132">
-        <f>H132/G132</f>
+        <f t="shared" si="8"/>
         <v>1.2790697674418605</v>
       </c>
       <c r="J132" t="b">
@@ -9993,7 +9963,7 @@
         <v>12</v>
       </c>
       <c r="B133" s="2" t="str">
-        <f>HYPERLINK(P133)</f>
+        <f t="shared" si="9"/>
         <v>https://iwp6.iwphys.org/animation/summer-physics/auto-impulse-compare.iwp</v>
       </c>
       <c r="D133" t="s">
@@ -10012,7 +9982,7 @@
         <v>14</v>
       </c>
       <c r="I133">
-        <f>H133/G133</f>
+        <f t="shared" si="8"/>
         <v>14</v>
       </c>
       <c r="J133" t="b">
@@ -10042,7 +10012,7 @@
         <v>12</v>
       </c>
       <c r="B134" s="2" t="str">
-        <f>HYPERLINK(P134)</f>
+        <f t="shared" si="9"/>
         <v>https://iwp6.iwphys.org/animation/summer-physics/collision-01.iwp</v>
       </c>
       <c r="D134" t="s">
@@ -10061,7 +10031,7 @@
         <v>3</v>
       </c>
       <c r="I134">
-        <f>H134/G134</f>
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
       <c r="J134" t="b">
@@ -10091,7 +10061,7 @@
         <v>12</v>
       </c>
       <c r="B135" s="2" t="str">
-        <f>HYPERLINK(P135)</f>
+        <f t="shared" si="9"/>
         <v>https://iwp6.iwphys.org/animation/summer-physics/collision-02.iwp</v>
       </c>
       <c r="D135" t="s">
@@ -10110,7 +10080,7 @@
         <v>3</v>
       </c>
       <c r="I135">
-        <f>H135/G135</f>
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
       <c r="J135" t="b">
@@ -10140,7 +10110,7 @@
         <v>12</v>
       </c>
       <c r="B136" s="2" t="str">
-        <f>HYPERLINK(P136)</f>
+        <f t="shared" si="9"/>
         <v>https://iwp6.iwphys.org/animation/summer-physics/collision-02b.iwp</v>
       </c>
       <c r="D136" t="s">
@@ -10159,7 +10129,7 @@
         <v>3</v>
       </c>
       <c r="I136">
-        <f>H136/G136</f>
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
       <c r="J136" t="b">
@@ -10189,7 +10159,7 @@
         <v>12</v>
       </c>
       <c r="B137" s="2" t="str">
-        <f>HYPERLINK(P137)</f>
+        <f t="shared" si="9"/>
         <v>https://iwp6.iwphys.org/animation/summer-physics/collision-03.iwp</v>
       </c>
       <c r="D137" t="s">
@@ -10208,7 +10178,7 @@
         <v>2</v>
       </c>
       <c r="I137">
-        <f>H137/G137</f>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="J137" t="b">
@@ -10238,7 +10208,7 @@
         <v>12</v>
       </c>
       <c r="B138" s="2" t="str">
-        <f>HYPERLINK(P138)</f>
+        <f t="shared" si="9"/>
         <v>https://iwp6.iwphys.org/animation/summer-physics/collision-04.iwp</v>
       </c>
       <c r="D138" t="s">
@@ -10257,7 +10227,7 @@
         <v>2</v>
       </c>
       <c r="I138">
-        <f>H138/G138</f>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="J138" t="b">
@@ -10287,7 +10257,7 @@
         <v>12</v>
       </c>
       <c r="B139" s="2" t="str">
-        <f>HYPERLINK(P139)</f>
+        <f t="shared" si="9"/>
         <v>https://iwp6.iwphys.org/animation/summer-physics/collision-elastic-2b.iwp</v>
       </c>
       <c r="D139" t="s">
@@ -10306,7 +10276,7 @@
         <v>3</v>
       </c>
       <c r="I139">
-        <f>H139/G139</f>
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
       <c r="J139" t="b">
@@ -10336,7 +10306,7 @@
         <v>12</v>
       </c>
       <c r="B140" s="2" t="str">
-        <f>HYPERLINK(P140)</f>
+        <f t="shared" si="9"/>
         <v>https://iwp6.iwphys.org/animation/summer-physics/collision-elastic-2d-01.iwp</v>
       </c>
       <c r="D140" t="s">
@@ -10355,7 +10325,7 @@
         <v>3</v>
       </c>
       <c r="I140">
-        <f>H140/G140</f>
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
       <c r="J140" t="b">
@@ -10385,7 +10355,7 @@
         <v>12</v>
       </c>
       <c r="B141" s="2" t="str">
-        <f>HYPERLINK(P141)</f>
+        <f t="shared" si="9"/>
         <v>https://iwp6.iwphys.org/animation/summer-physics/collision-elastic-3.iwp</v>
       </c>
       <c r="D141" t="s">
@@ -10404,7 +10374,7 @@
         <v>3</v>
       </c>
       <c r="I141">
-        <f>H141/G141</f>
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
       <c r="J141" t="b">
@@ -10434,7 +10404,7 @@
         <v>12</v>
       </c>
       <c r="B142" s="2" t="str">
-        <f>HYPERLINK(P142)</f>
+        <f t="shared" si="9"/>
         <v>https://iwp6.iwphys.org/animation/summer-physics/collision-elastic-4a.iwp</v>
       </c>
       <c r="D142" t="s">
@@ -10453,7 +10423,7 @@
         <v>2</v>
       </c>
       <c r="I142">
-        <f>H142/G142</f>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="J142" t="b">
@@ -10483,7 +10453,7 @@
         <v>12</v>
       </c>
       <c r="B143" s="2" t="str">
-        <f>HYPERLINK(P143)</f>
+        <f t="shared" si="9"/>
         <v>https://iwp6.iwphys.org/animation/summer-physics/collision-explosion-02.iwp</v>
       </c>
       <c r="D143" t="s">
@@ -10502,7 +10472,7 @@
         <v>10</v>
       </c>
       <c r="I143">
-        <f>H143/G143</f>
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J143" t="b">
@@ -10532,7 +10502,7 @@
         <v>12</v>
       </c>
       <c r="B144" s="2" t="str">
-        <f>HYPERLINK(P144)</f>
+        <f t="shared" si="9"/>
         <v>https://iwp6.iwphys.org/animation/summer-physics/collision-explosion-02b.iwp</v>
       </c>
       <c r="D144" t="s">
@@ -10551,7 +10521,7 @@
         <v>10</v>
       </c>
       <c r="I144">
-        <f>H144/G144</f>
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J144" t="b">
@@ -10581,7 +10551,7 @@
         <v>12</v>
       </c>
       <c r="B145" s="2" t="str">
-        <f>HYPERLINK(P145)</f>
+        <f t="shared" si="9"/>
         <v>https://iwp6.iwphys.org/animation/summer-physics/collision-inelastic-06.iwp</v>
       </c>
       <c r="D145" t="s">
@@ -10600,7 +10570,7 @@
         <v>2</v>
       </c>
       <c r="I145">
-        <f>H145/G145</f>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="J145" t="b">
@@ -10630,7 +10600,7 @@
         <v>12</v>
       </c>
       <c r="B146" s="2" t="str">
-        <f>HYPERLINK(P146)</f>
+        <f t="shared" si="9"/>
         <v>https://iwp6.iwphys.org/animation/summer-physics/eforce-05.iwp</v>
       </c>
       <c r="D146" t="s">
@@ -10678,7 +10648,7 @@
         <v>12</v>
       </c>
       <c r="B147" s="2" t="str">
-        <f>HYPERLINK(P147)</f>
+        <f t="shared" si="9"/>
         <v>https://iwp6.iwphys.org/animation/summer-physics/eforce-07.iwp</v>
       </c>
       <c r="D147" t="s">
@@ -10726,7 +10696,7 @@
         <v>12</v>
       </c>
       <c r="B148" s="2" t="str">
-        <f>HYPERLINK(P148)</f>
+        <f t="shared" si="9"/>
         <v>https://iwp6.iwphys.org/animation/summer-physics/eforce-08.iwp</v>
       </c>
       <c r="D148" t="s">
@@ -10775,7 +10745,7 @@
         <v>12</v>
       </c>
       <c r="B149" s="2" t="str">
-        <f>HYPERLINK(P149)</f>
+        <f t="shared" si="9"/>
         <v>https://iwp6.iwphys.org/animation/summer-physics/eforce-09.iwp</v>
       </c>
       <c r="D149" t="s">
@@ -10824,7 +10794,7 @@
         <v>12</v>
       </c>
       <c r="B150" s="2" t="str">
-        <f>HYPERLINK(P150)</f>
+        <f t="shared" si="9"/>
         <v>https://iwp6.iwphys.org/animation/summer-physics/energy-spring-1b.iwp</v>
       </c>
       <c r="D150" t="s">
@@ -10873,7 +10843,7 @@
         <v>12</v>
       </c>
       <c r="B151" s="2" t="str">
-        <f>HYPERLINK(P151)</f>
+        <f t="shared" si="9"/>
         <v>https://iwp6.iwphys.org/animation/summer-physics/energy-vertspring-01.iwp</v>
       </c>
       <c r="D151" t="s">
@@ -10922,7 +10892,7 @@
         <v>12</v>
       </c>
       <c r="B152" s="2" t="str">
-        <f>HYPERLINK(P152)</f>
+        <f t="shared" si="9"/>
         <v>https://iwp6.iwphys.org/animation/summer-physics/equilibrium-01.iwp</v>
       </c>
       <c r="D152" t="s">
@@ -10970,7 +10940,7 @@
         <v>12</v>
       </c>
       <c r="B153" s="2" t="str">
-        <f>HYPERLINK(P153)</f>
+        <f t="shared" si="9"/>
         <v>https://iwp6.iwphys.org/animation/summer-physics/equilibrium-02.iwp</v>
       </c>
       <c r="D153" t="s">
@@ -10989,7 +10959,7 @@
         <v>6</v>
       </c>
       <c r="I153">
-        <f>H153/G153</f>
+        <f t="shared" ref="I153:I173" si="10">H153/G153</f>
         <v>6</v>
       </c>
       <c r="J153" t="b">
@@ -11019,7 +10989,7 @@
         <v>12</v>
       </c>
       <c r="B154" s="2" t="str">
-        <f>HYPERLINK(P154)</f>
+        <f t="shared" si="9"/>
         <v>https://iwp6.iwphys.org/animation/summer-physics/friction01b.iwp</v>
       </c>
       <c r="D154" t="s">
@@ -11038,7 +11008,7 @@
         <v>2</v>
       </c>
       <c r="I154">
-        <f>H154/G154</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="J154" t="b">
@@ -11068,7 +11038,7 @@
         <v>12</v>
       </c>
       <c r="B155" s="2" t="str">
-        <f>HYPERLINK(P155)</f>
+        <f t="shared" si="9"/>
         <v>https://iwp6.iwphys.org/animation/summer-physics/friction01c.iwp</v>
       </c>
       <c r="D155" t="s">
@@ -11087,7 +11057,7 @@
         <v>6</v>
       </c>
       <c r="I155">
-        <f>H155/G155</f>
+        <f t="shared" si="10"/>
         <v>3</v>
       </c>
       <c r="J155" t="b">
@@ -11117,7 +11087,7 @@
         <v>12</v>
       </c>
       <c r="B156" s="2" t="str">
-        <f>HYPERLINK(P156)</f>
+        <f t="shared" si="9"/>
         <v>https://iwp6.iwphys.org/animation/summer-physics/gravitation-01b.iwp</v>
       </c>
       <c r="D156" t="s">
@@ -11136,7 +11106,7 @@
         <v>4</v>
       </c>
       <c r="I156">
-        <f>H156/G156</f>
+        <f t="shared" si="10"/>
         <v>4</v>
       </c>
       <c r="J156" t="b">
@@ -11166,7 +11136,7 @@
         <v>12</v>
       </c>
       <c r="B157" s="2" t="str">
-        <f>HYPERLINK(P157)</f>
+        <f t="shared" si="9"/>
         <v>https://iwp6.iwphys.org/animation/summer-physics/gravitation-01e.iwp</v>
       </c>
       <c r="D157" t="s">
@@ -11185,7 +11155,7 @@
         <v>12</v>
       </c>
       <c r="I157">
-        <f>H157/G157</f>
+        <f t="shared" si="10"/>
         <v>12</v>
       </c>
       <c r="J157" t="b">
@@ -11215,7 +11185,7 @@
         <v>12</v>
       </c>
       <c r="B158" s="2" t="str">
-        <f>HYPERLINK(P158)</f>
+        <f t="shared" si="9"/>
         <v>https://iwp6.iwphys.org/animation/summer-physics/gravitation-02b.iwp</v>
       </c>
       <c r="D158" t="s">
@@ -11234,7 +11204,7 @@
         <v>2</v>
       </c>
       <c r="I158">
-        <f>H158/G158</f>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="J158" t="b">
@@ -11264,7 +11234,7 @@
         <v>12</v>
       </c>
       <c r="B159" s="2" t="str">
-        <f>HYPERLINK(P159)</f>
+        <f t="shared" si="9"/>
         <v>https://iwp6.iwphys.org/animation/summer-physics/nsl-00.iwp</v>
       </c>
       <c r="D159" t="s">
@@ -11283,7 +11253,7 @@
         <v>202</v>
       </c>
       <c r="I159">
-        <f>H159/G159</f>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="J159" t="b">
@@ -11313,7 +11283,7 @@
         <v>12</v>
       </c>
       <c r="B160" s="2" t="str">
-        <f>HYPERLINK(P160)</f>
+        <f t="shared" si="9"/>
         <v>https://iwp6.iwphys.org/animation/summer-physics/nsl-01.iwp</v>
       </c>
       <c r="D160" t="s">
@@ -11332,7 +11302,7 @@
         <v>101</v>
       </c>
       <c r="I160">
-        <f>H160/G160</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="J160" t="b">
@@ -11362,7 +11332,7 @@
         <v>12</v>
       </c>
       <c r="B161" s="2" t="str">
-        <f>HYPERLINK(P161)</f>
+        <f t="shared" si="9"/>
         <v>https://iwp6.iwphys.org/animation/summer-physics/nsl-02.iwp</v>
       </c>
       <c r="D161" t="s">
@@ -11381,7 +11351,7 @@
         <v>101</v>
       </c>
       <c r="I161">
-        <f>H161/G161</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="J161" t="b">
@@ -11411,7 +11381,7 @@
         <v>12</v>
       </c>
       <c r="B162" s="2" t="str">
-        <f>HYPERLINK(P162)</f>
+        <f t="shared" si="9"/>
         <v>https://iwp6.iwphys.org/animation/summer-physics/pendulum02b.iwp</v>
       </c>
       <c r="D162" t="s">
@@ -11430,7 +11400,7 @@
         <v>24757</v>
       </c>
       <c r="I162">
-        <f>H162/G162</f>
+        <f t="shared" si="10"/>
         <v>24.757000000000001</v>
       </c>
       <c r="J162" t="b">
@@ -11460,7 +11430,7 @@
         <v>12</v>
       </c>
       <c r="B163" s="2" t="str">
-        <f>HYPERLINK(P163)</f>
+        <f t="shared" si="9"/>
         <v>https://iwp6.iwphys.org/animation/summer-physics/pendulum03.iwp</v>
       </c>
       <c r="D163" t="s">
@@ -11479,7 +11449,7 @@
         <v>12925</v>
       </c>
       <c r="I163">
-        <f>H163/G163</f>
+        <f t="shared" si="10"/>
         <v>12.925000000000001</v>
       </c>
       <c r="J163" t="b">
@@ -11509,7 +11479,7 @@
         <v>12</v>
       </c>
       <c r="B164" s="2" t="str">
-        <f>HYPERLINK(P164)</f>
+        <f t="shared" si="9"/>
         <v>https://iwp6.iwphys.org/animation/summer-physics/proj-vect-00.iwp</v>
       </c>
       <c r="D164" t="s">
@@ -11528,7 +11498,7 @@
         <v>107</v>
       </c>
       <c r="I164">
-        <f>H164/G164</f>
+        <f t="shared" si="10"/>
         <v>1.0594059405940595</v>
       </c>
       <c r="J164" t="b">
@@ -11558,7 +11528,7 @@
         <v>12</v>
       </c>
       <c r="B165" s="2" t="str">
-        <f>HYPERLINK(P165)</f>
+        <f t="shared" si="9"/>
         <v>https://iwp6.iwphys.org/animation/summer-physics/projectile-compare-1.iwp</v>
       </c>
       <c r="D165" t="s">
@@ -11577,7 +11547,7 @@
         <v>6</v>
       </c>
       <c r="I165">
-        <f>H165/G165</f>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
       <c r="J165" t="b">
@@ -11607,7 +11577,7 @@
         <v>12</v>
       </c>
       <c r="B166" s="2" t="str">
-        <f>HYPERLINK(P166)</f>
+        <f t="shared" si="9"/>
         <v>https://iwp6.iwphys.org/animation/summer-physics/projectile-problem-2.iwp</v>
       </c>
       <c r="D166" t="s">
@@ -11626,7 +11596,7 @@
         <v>2</v>
       </c>
       <c r="I166">
-        <f>H166/G166</f>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="J166" t="b">
@@ -11656,7 +11626,7 @@
         <v>12</v>
       </c>
       <c r="B167" s="2" t="str">
-        <f>HYPERLINK(P167)</f>
+        <f t="shared" si="9"/>
         <v>https://iwp6.iwphys.org/animation/summer-physics/projectile-problem-3.iwp</v>
       </c>
       <c r="D167" t="s">
@@ -11675,7 +11645,7 @@
         <v>2</v>
       </c>
       <c r="I167">
-        <f>H167/G167</f>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="J167" t="b">
@@ -11705,7 +11675,7 @@
         <v>12</v>
       </c>
       <c r="B168" s="2" t="str">
-        <f>HYPERLINK(P168)</f>
+        <f t="shared" si="9"/>
         <v>https://iwp6.iwphys.org/animation/summer-physics/shm-phase-02b.iwp</v>
       </c>
       <c r="D168" t="s">
@@ -11724,7 +11694,7 @@
         <v>4</v>
       </c>
       <c r="I168">
-        <f>H168/G168</f>
+        <f t="shared" si="10"/>
         <v>4</v>
       </c>
       <c r="J168" t="b">
@@ -11754,7 +11724,7 @@
         <v>12</v>
       </c>
       <c r="B169" s="2" t="str">
-        <f>HYPERLINK(P169)</f>
+        <f t="shared" si="9"/>
         <v>https://iwp6.iwphys.org/animation/summer-physics/spring-circle-analogy-02.iwp</v>
       </c>
       <c r="D169" t="s">
@@ -11773,7 +11743,7 @@
         <v>20</v>
       </c>
       <c r="I169">
-        <f>H169/G169</f>
+        <f t="shared" si="10"/>
         <v>20</v>
       </c>
       <c r="J169" t="b">
@@ -11803,7 +11773,7 @@
         <v>12</v>
       </c>
       <c r="B170" s="2" t="str">
-        <f>HYPERLINK(P170)</f>
+        <f t="shared" si="9"/>
         <v>https://iwp6.iwphys.org/animation/summer-physics/spring-equation-02.iwp</v>
       </c>
       <c r="D170" t="s">
@@ -11822,7 +11792,7 @@
         <v>7</v>
       </c>
       <c r="I170">
-        <f>H170/G170</f>
+        <f t="shared" si="10"/>
         <v>7</v>
       </c>
       <c r="J170" t="b">
@@ -11852,7 +11822,7 @@
         <v>12</v>
       </c>
       <c r="B171" s="2" t="str">
-        <f>HYPERLINK(P171)</f>
+        <f t="shared" si="9"/>
         <v>https://iwp6.iwphys.org/animation/summer-physics/spring-equation-03.iwp</v>
       </c>
       <c r="D171" t="s">
@@ -11871,7 +11841,7 @@
         <v>7</v>
       </c>
       <c r="I171">
-        <f>H171/G171</f>
+        <f t="shared" si="10"/>
         <v>7</v>
       </c>
       <c r="J171" t="b">
@@ -11901,7 +11871,7 @@
         <v>12</v>
       </c>
       <c r="B172" s="2" t="str">
-        <f>HYPERLINK(P172)</f>
+        <f t="shared" si="9"/>
         <v>https://iwp6.iwphys.org/animation/summer-physics/spring-equation-04.iwp</v>
       </c>
       <c r="D172" t="s">
@@ -11920,7 +11890,7 @@
         <v>7</v>
       </c>
       <c r="I172">
-        <f>H172/G172</f>
+        <f t="shared" si="10"/>
         <v>7</v>
       </c>
       <c r="J172" t="b">
@@ -11950,7 +11920,7 @@
         <v>12</v>
       </c>
       <c r="B173" s="2" t="str">
-        <f>HYPERLINK(P173)</f>
+        <f t="shared" si="9"/>
         <v>https://iwp6.iwphys.org/animation/summer-physics/spring-motion-4.iwp</v>
       </c>
       <c r="D173" t="s">
@@ -11969,7 +11939,7 @@
         <v>9</v>
       </c>
       <c r="I173">
-        <f>H173/G173</f>
+        <f t="shared" si="10"/>
         <v>9</v>
       </c>
       <c r="J173" t="b">
@@ -11999,7 +11969,7 @@
         <v>12</v>
       </c>
       <c r="B174" s="2" t="str">
-        <f>HYPERLINK(P174)</f>
+        <f t="shared" si="9"/>
         <v>https://iwp6.iwphys.org/animation/summer-physics/stopblock01c.iwp</v>
       </c>
       <c r="D174" t="s">
@@ -12047,7 +12017,7 @@
         <v>12</v>
       </c>
       <c r="B175" s="2" t="str">
-        <f>HYPERLINK(P175)</f>
+        <f t="shared" si="9"/>
         <v>https://iwp6.iwphys.org/animation/summer-physics/stopblock01f.iwp</v>
       </c>
       <c r="D175" t="s">
@@ -12096,7 +12066,7 @@
         <v>12</v>
       </c>
       <c r="B176" s="2" t="str">
-        <f>HYPERLINK(P176)</f>
+        <f t="shared" si="9"/>
         <v>https://iwp6.iwphys.org/animation/summer-physics/vector02.iwp</v>
       </c>
       <c r="D176" t="s">
@@ -12144,7 +12114,7 @@
         <v>12</v>
       </c>
       <c r="B177" s="2" t="str">
-        <f>HYPERLINK(P177)</f>
+        <f t="shared" si="9"/>
         <v>https://iwp6.iwphys.org/animation/summer-physics/vector03.iwp</v>
       </c>
       <c r="D177" t="s">
@@ -12192,7 +12162,7 @@
         <v>12</v>
       </c>
       <c r="B178" s="2" t="str">
-        <f>HYPERLINK(P178)</f>
+        <f t="shared" si="9"/>
         <v>https://iwp6.iwphys.org/animation/summer-physics/vector04.iwp</v>
       </c>
       <c r="D178" t="s">
@@ -12240,7 +12210,7 @@
         <v>12</v>
       </c>
       <c r="B179" s="2" t="str">
-        <f>HYPERLINK(P179)</f>
+        <f t="shared" si="9"/>
         <v>https://iwp6.iwphys.org/animation/summer-physics/velocity01b.iwp</v>
       </c>
       <c r="D179" t="s">
@@ -12259,7 +12229,7 @@
         <v>4</v>
       </c>
       <c r="I179">
-        <f>H179/G179</f>
+        <f t="shared" ref="I179:I184" si="11">H179/G179</f>
         <v>4</v>
       </c>
       <c r="J179" t="b">
@@ -12289,7 +12259,7 @@
         <v>12</v>
       </c>
       <c r="B180" s="2" t="str">
-        <f>HYPERLINK(P180)</f>
+        <f t="shared" si="9"/>
         <v>https://iwp6.iwphys.org/animation/summer-physics/velocity02b.iwp</v>
       </c>
       <c r="D180" t="s">
@@ -12308,7 +12278,7 @@
         <v>4</v>
       </c>
       <c r="I180">
-        <f>H180/G180</f>
+        <f t="shared" si="11"/>
         <v>4</v>
       </c>
       <c r="J180" t="b">
@@ -12338,7 +12308,7 @@
         <v>12</v>
       </c>
       <c r="B181" s="2" t="str">
-        <f>HYPERLINK(P181)</f>
+        <f t="shared" si="9"/>
         <v>https://iwp6.iwphys.org/animation/summer-physics/velocity04.iwp</v>
       </c>
       <c r="D181" t="s">
@@ -12357,7 +12327,7 @@
         <v>4</v>
       </c>
       <c r="I181">
-        <f>H181/G181</f>
+        <f t="shared" si="11"/>
         <v>4</v>
       </c>
       <c r="J181" t="b">
@@ -12387,7 +12357,7 @@
         <v>12</v>
       </c>
       <c r="B182" s="2" t="str">
-        <f>HYPERLINK(P182)</f>
+        <f t="shared" si="9"/>
         <v>https://iwp6.iwphys.org/animation/summer-physics/velocity06.iwp</v>
       </c>
       <c r="D182" t="s">
@@ -12406,7 +12376,7 @@
         <v>381</v>
       </c>
       <c r="I182">
-        <f>H182/G182</f>
+        <f t="shared" si="11"/>
         <v>7.4705882352941178</v>
       </c>
       <c r="J182" t="b">
@@ -12436,7 +12406,7 @@
         <v>12</v>
       </c>
       <c r="B183" s="2" t="str">
-        <f>HYPERLINK(P183)</f>
+        <f t="shared" si="9"/>
         <v>https://iwp6.iwphys.org/animation/summer-physics/work-01.iwp</v>
       </c>
       <c r="D183" t="s">
@@ -12455,7 +12425,7 @@
         <v>205</v>
       </c>
       <c r="I183">
-        <f>H183/G183</f>
+        <f t="shared" si="11"/>
         <v>3.253968253968254</v>
       </c>
       <c r="J183" t="b">
@@ -12485,7 +12455,7 @@
         <v>12</v>
       </c>
       <c r="B184" s="2" t="str">
-        <f>HYPERLINK(P184)</f>
+        <f t="shared" si="9"/>
         <v>https://iwp6.iwphys.org/animation/unit-test-2017/TEST_Euler_SelfReference.iwp</v>
       </c>
       <c r="D184" t="s">
@@ -12504,7 +12474,7 @@
         <v>2</v>
       </c>
       <c r="I184">
-        <f>H184/G184</f>
+        <f t="shared" si="11"/>
         <v>2</v>
       </c>
       <c r="J184" t="b">
@@ -12534,7 +12504,7 @@
         <v>12</v>
       </c>
       <c r="B185" s="2" t="str">
-        <f>HYPERLINK(P185)</f>
+        <f t="shared" si="9"/>
         <v>https://iwp6.iwphys.org/animation/unit-test-2017/TEST_euler.iwp</v>
       </c>
       <c r="D185" t="s">
@@ -12582,7 +12552,7 @@
         <v>12</v>
       </c>
       <c r="B186" s="2" t="str">
-        <f>HYPERLINK(P186)</f>
+        <f t="shared" si="9"/>
         <v>https://iwp6.iwphys.org/animation/winters-ncssm-2009/beats.iwp</v>
       </c>
       <c r="D186" t="s">
@@ -12631,7 +12601,7 @@
         <v>12</v>
       </c>
       <c r="B187" s="2" t="str">
-        <f>HYPERLINK(P187)</f>
+        <f t="shared" si="9"/>
         <v>https://iwp6.iwphys.org/animation/winters-ncssm-2009/capacitor-discharge.iwp</v>
       </c>
       <c r="D187" t="s">
@@ -12680,7 +12650,7 @@
         <v>12</v>
       </c>
       <c r="B188" s="2" t="str">
-        <f>HYPERLINK(P188)</f>
+        <f t="shared" si="9"/>
         <v>https://iwp6.iwphys.org/animation/winters-ncssm-2009/clock-02.iwp</v>
       </c>
       <c r="D188" t="s">
@@ -12728,7 +12698,7 @@
         <v>12</v>
       </c>
       <c r="B189" s="2" t="str">
-        <f>HYPERLINK(P189)</f>
+        <f t="shared" si="9"/>
         <v>https://iwp6.iwphys.org/animation/winters-ncssm-2009/collision-04.iwp</v>
       </c>
       <c r="D189" t="s">
@@ -12747,7 +12717,7 @@
         <v>2</v>
       </c>
       <c r="I189">
-        <f>H189/G189</f>
+        <f t="shared" ref="I189:I196" si="12">H189/G189</f>
         <v>2</v>
       </c>
       <c r="J189" t="b">
@@ -12777,7 +12747,7 @@
         <v>12</v>
       </c>
       <c r="B190" s="2" t="str">
-        <f>HYPERLINK(P190)</f>
+        <f t="shared" si="9"/>
         <v>https://iwp6.iwphys.org/animation/winters-ncssm-2009/collision-elastic-2d-template.iwp</v>
       </c>
       <c r="D190" t="s">
@@ -12796,7 +12766,7 @@
         <v>3</v>
       </c>
       <c r="I190">
-        <f>H190/G190</f>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="J190" t="b">
@@ -12826,7 +12796,7 @@
         <v>12</v>
       </c>
       <c r="B191" s="2" t="str">
-        <f>HYPERLINK(P191)</f>
+        <f t="shared" si="9"/>
         <v>https://iwp6.iwphys.org/animation/winters-ncssm-2009/collision-inelastic-2d-01.iwp</v>
       </c>
       <c r="D191" t="s">
@@ -12845,7 +12815,7 @@
         <v>5</v>
       </c>
       <c r="I191">
-        <f>H191/G191</f>
+        <f t="shared" si="12"/>
         <v>5</v>
       </c>
       <c r="J191" t="b">
@@ -12875,7 +12845,7 @@
         <v>12</v>
       </c>
       <c r="B192" s="2" t="str">
-        <f>HYPERLINK(P192)</f>
+        <f t="shared" si="9"/>
         <v>https://iwp6.iwphys.org/animation/winters-ncssm-2009/compton-02.iwp</v>
       </c>
       <c r="D192" t="s">
@@ -12894,7 +12864,7 @@
         <v>1886</v>
       </c>
       <c r="I192">
-        <f>H192/G192</f>
+        <f t="shared" si="12"/>
         <v>2.0411255411255413</v>
       </c>
       <c r="J192" t="b">
@@ -12924,7 +12894,7 @@
         <v>12</v>
       </c>
       <c r="B193" s="2" t="str">
-        <f>HYPERLINK(P193)</f>
+        <f t="shared" si="9"/>
         <v>https://iwp6.iwphys.org/animation/winters-ncssm-2009/compton-03.iwp</v>
       </c>
       <c r="D193" t="s">
@@ -12943,7 +12913,7 @@
         <v>732</v>
       </c>
       <c r="I193">
-        <f>H193/G193</f>
+        <f t="shared" si="12"/>
         <v>2.172106824925816</v>
       </c>
       <c r="J193" t="b">
@@ -12973,7 +12943,7 @@
         <v>12</v>
       </c>
       <c r="B194" s="2" t="str">
-        <f>HYPERLINK(P194)</f>
+        <f t="shared" ref="B194:B227" si="13">HYPERLINK(P194)</f>
         <v>https://iwp6.iwphys.org/animation/winters-ncssm-2009/coulombslaw01.iwp</v>
       </c>
       <c r="D194" t="s">
@@ -12992,7 +12962,7 @@
         <v>5</v>
       </c>
       <c r="I194">
-        <f>H194/G194</f>
+        <f t="shared" si="12"/>
         <v>5</v>
       </c>
       <c r="J194" t="b">
@@ -13022,7 +12992,7 @@
         <v>12</v>
       </c>
       <c r="B195" s="2" t="str">
-        <f>HYPERLINK(P195)</f>
+        <f t="shared" si="13"/>
         <v>https://iwp6.iwphys.org/animation/winters-ncssm-2009/doppler3.iwp</v>
       </c>
       <c r="D195" t="s">
@@ -13041,7 +13011,7 @@
         <v>1</v>
       </c>
       <c r="I195">
-        <f>H195/G195</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="J195" t="b">
@@ -13071,7 +13041,7 @@
         <v>12</v>
       </c>
       <c r="B196" s="2" t="str">
-        <f>HYPERLINK(P196)</f>
+        <f t="shared" si="13"/>
         <v>https://iwp6.iwphys.org/animation/winters-ncssm-2009/dvat-11.iwp</v>
       </c>
       <c r="D196" t="s">
@@ -13090,7 +13060,7 @@
         <v>2</v>
       </c>
       <c r="I196">
-        <f>H196/G196</f>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="J196" t="b">
@@ -13120,7 +13090,7 @@
         <v>12</v>
       </c>
       <c r="B197" s="2" t="str">
-        <f>HYPERLINK(P197)</f>
+        <f t="shared" si="13"/>
         <v>https://iwp6.iwphys.org/animation/winters-ncssm-2009/empath3.iwp</v>
       </c>
       <c r="D197" t="s">
@@ -13168,7 +13138,7 @@
         <v>12</v>
       </c>
       <c r="B198" s="2" t="str">
-        <f>HYPERLINK(P198)</f>
+        <f t="shared" si="13"/>
         <v>https://iwp6.iwphys.org/animation/winters-ncssm-2009/epotential-02c2.iwp</v>
       </c>
       <c r="D198" t="s">
@@ -13216,7 +13186,7 @@
         <v>12</v>
       </c>
       <c r="B199" s="2" t="str">
-        <f>HYPERLINK(P199)</f>
+        <f t="shared" si="13"/>
         <v>https://iwp6.iwphys.org/animation/winters-ncssm-2009/epotential-02h.iwp</v>
       </c>
       <c r="D199" t="s">
@@ -13264,7 +13234,7 @@
         <v>12</v>
       </c>
       <c r="B200" s="2" t="str">
-        <f>HYPERLINK(P200)</f>
+        <f t="shared" si="13"/>
         <v>https://iwp6.iwphys.org/animation/winters-ncssm-2009/epotential-02i.iwp</v>
       </c>
       <c r="D200" t="s">
@@ -13312,7 +13282,7 @@
         <v>12</v>
       </c>
       <c r="B201" s="2" t="str">
-        <f>HYPERLINK(P201)</f>
+        <f t="shared" si="13"/>
         <v>https://iwp6.iwphys.org/animation/winters-ncssm-2009/equilibrium-03b.iwp</v>
       </c>
       <c r="D201" t="s">
@@ -13331,7 +13301,7 @@
         <v>6</v>
       </c>
       <c r="I201">
-        <f>H201/G201</f>
+        <f t="shared" ref="I201:I206" si="14">H201/G201</f>
         <v>6</v>
       </c>
       <c r="J201" t="b">
@@ -13361,7 +13331,7 @@
         <v>12</v>
       </c>
       <c r="B202" s="2" t="str">
-        <f>HYPERLINK(P202)</f>
+        <f t="shared" si="13"/>
         <v>https://iwp6.iwphys.org/animation/winters-ncssm-2009/fluid-dynamics-torricelli-01.iwp</v>
       </c>
       <c r="D202" t="s">
@@ -13380,7 +13350,7 @@
         <v>10</v>
       </c>
       <c r="I202">
-        <f>H202/G202</f>
+        <f t="shared" si="14"/>
         <v>10</v>
       </c>
       <c r="J202" t="b">
@@ -13410,7 +13380,7 @@
         <v>12</v>
       </c>
       <c r="B203" s="2" t="str">
-        <f>HYPERLINK(P203)</f>
+        <f t="shared" si="13"/>
         <v>https://iwp6.iwphys.org/animation/winters-ncssm-2009/kingraph1.iwp</v>
       </c>
       <c r="D203" t="s">
@@ -13429,7 +13399,7 @@
         <v>2</v>
       </c>
       <c r="I203">
-        <f>H203/G203</f>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="J203" t="b">
@@ -13459,7 +13429,7 @@
         <v>12</v>
       </c>
       <c r="B204" s="2" t="str">
-        <f>HYPERLINK(P204)</f>
+        <f t="shared" si="13"/>
         <v>https://iwp6.iwphys.org/animation/winters-ncssm-2009/L00-2d.iwp</v>
       </c>
       <c r="D204" t="s">
@@ -13478,7 +13448,7 @@
         <v>2</v>
       </c>
       <c r="I204">
-        <f>H204/G204</f>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="J204" t="b">
@@ -13508,7 +13478,7 @@
         <v>12</v>
       </c>
       <c r="B205" s="2" t="str">
-        <f>HYPERLINK(P205)</f>
+        <f t="shared" si="13"/>
         <v>https://iwp6.iwphys.org/animation/winters-ncssm-2009/L00-3b.iwp</v>
       </c>
       <c r="D205" t="s">
@@ -13527,7 +13497,7 @@
         <v>4</v>
       </c>
       <c r="I205">
-        <f>H205/G205</f>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="J205" t="b">
@@ -13557,7 +13527,7 @@
         <v>12</v>
       </c>
       <c r="B206" s="2" t="str">
-        <f>HYPERLINK(P206)</f>
+        <f t="shared" si="13"/>
         <v>https://iwp6.iwphys.org/animation/winters-ncssm-2009/lens-ray-tracing.iwp</v>
       </c>
       <c r="D206" t="s">
@@ -13576,7 +13546,7 @@
         <v>6</v>
       </c>
       <c r="I206">
-        <f>H206/G206</f>
+        <f t="shared" si="14"/>
         <v>6</v>
       </c>
       <c r="J206" t="b">
@@ -13606,7 +13576,7 @@
         <v>12</v>
       </c>
       <c r="B207" s="2" t="str">
-        <f>HYPERLINK(P207)</f>
+        <f t="shared" si="13"/>
         <v>https://iwp6.iwphys.org/animation/winters-ncssm-2009/modulo-cockrell.iwp</v>
       </c>
       <c r="D207" t="s">
@@ -13654,7 +13624,7 @@
         <v>12</v>
       </c>
       <c r="B208" s="2" t="str">
-        <f>HYPERLINK(P208)</f>
+        <f t="shared" si="13"/>
         <v>https://iwp6.iwphys.org/animation/winters-ncssm-2009/pendulum02b.iwp</v>
       </c>
       <c r="D208" t="s">
@@ -13673,7 +13643,7 @@
         <v>24757</v>
       </c>
       <c r="I208">
-        <f>H208/G208</f>
+        <f t="shared" ref="I208:I221" si="15">H208/G208</f>
         <v>24.757000000000001</v>
       </c>
       <c r="J208" t="b">
@@ -13703,7 +13673,7 @@
         <v>12</v>
       </c>
       <c r="B209" s="2" t="str">
-        <f>HYPERLINK(P209)</f>
+        <f t="shared" si="13"/>
         <v>https://iwp6.iwphys.org/animation/winters-ncssm-2009/rot-kin-02.iwp</v>
       </c>
       <c r="D209" t="s">
@@ -13722,7 +13692,7 @@
         <v>12</v>
       </c>
       <c r="I209">
-        <f>H209/G209</f>
+        <f t="shared" si="15"/>
         <v>12</v>
       </c>
       <c r="J209" t="b">
@@ -13752,7 +13722,7 @@
         <v>12</v>
       </c>
       <c r="B210" s="2" t="str">
-        <f>HYPERLINK(P210)</f>
+        <f t="shared" si="13"/>
         <v>https://iwp6.iwphys.org/animation/winters-ncssm-2009/rot-kin-03.iwp</v>
       </c>
       <c r="D210" t="s">
@@ -13771,7 +13741,7 @@
         <v>8</v>
       </c>
       <c r="I210">
-        <f>H210/G210</f>
+        <f t="shared" si="15"/>
         <v>8</v>
       </c>
       <c r="J210" t="b">
@@ -13801,7 +13771,7 @@
         <v>12</v>
       </c>
       <c r="B211" s="2" t="str">
-        <f>HYPERLINK(P211)</f>
+        <f t="shared" si="13"/>
         <v>https://iwp6.iwphys.org/animation/winters-ncssm-2009/shm-phase-01.iwp</v>
       </c>
       <c r="D211" t="s">
@@ -13820,7 +13790,7 @@
         <v>4</v>
       </c>
       <c r="I211">
-        <f>H211/G211</f>
+        <f t="shared" si="15"/>
         <v>4</v>
       </c>
       <c r="J211" t="b">
@@ -13850,7 +13820,7 @@
         <v>12</v>
       </c>
       <c r="B212" s="2" t="str">
-        <f>HYPERLINK(P212)</f>
+        <f t="shared" si="13"/>
         <v>https://iwp6.iwphys.org/animation/winters-ncssm-2009/shm-phase-02.iwp</v>
       </c>
       <c r="D212" t="s">
@@ -13869,7 +13839,7 @@
         <v>4</v>
       </c>
       <c r="I212">
-        <f>H212/G212</f>
+        <f t="shared" si="15"/>
         <v>4</v>
       </c>
       <c r="J212" t="b">
@@ -13899,7 +13869,7 @@
         <v>12</v>
       </c>
       <c r="B213" s="2" t="str">
-        <f>HYPERLINK(P213)</f>
+        <f t="shared" si="13"/>
         <v>https://iwp6.iwphys.org/animation/winters-ncssm-2009/shm-synchronize-02.iwp</v>
       </c>
       <c r="D213" t="s">
@@ -13918,7 +13888,7 @@
         <v>2</v>
       </c>
       <c r="I213">
-        <f>H213/G213</f>
+        <f t="shared" si="15"/>
         <v>2</v>
       </c>
       <c r="J213" t="b">
@@ -13948,7 +13918,7 @@
         <v>12</v>
       </c>
       <c r="B214" s="2" t="str">
-        <f>HYPERLINK(P214)</f>
+        <f t="shared" si="13"/>
         <v>https://iwp6.iwphys.org/animation/winters-ncssm-2009/slot-view-01b.iwp</v>
       </c>
       <c r="D214" t="s">
@@ -13967,7 +13937,7 @@
         <v>11</v>
       </c>
       <c r="I214">
-        <f>H214/G214</f>
+        <f t="shared" si="15"/>
         <v>11</v>
       </c>
       <c r="J214" t="b">
@@ -13997,7 +13967,7 @@
         <v>12</v>
       </c>
       <c r="B215" s="2" t="str">
-        <f>HYPERLINK(P215)</f>
+        <f t="shared" si="13"/>
         <v>https://iwp6.iwphys.org/animation/winters-ncssm-2009/spring-circle-analogy-02.iwp</v>
       </c>
       <c r="D215" t="s">
@@ -14016,7 +13986,7 @@
         <v>20</v>
       </c>
       <c r="I215">
-        <f>H215/G215</f>
+        <f t="shared" si="15"/>
         <v>20</v>
       </c>
       <c r="J215" t="b">
@@ -14046,7 +14016,7 @@
         <v>12</v>
       </c>
       <c r="B216" s="2" t="str">
-        <f>HYPERLINK(P216)</f>
+        <f t="shared" si="13"/>
         <v>https://iwp6.iwphys.org/animation/winters-ncssm-2009/spring-motion-02.iwp</v>
       </c>
       <c r="D216" t="s">
@@ -14065,7 +14035,7 @@
         <v>41</v>
       </c>
       <c r="I216">
-        <f>H216/G216</f>
+        <f t="shared" si="15"/>
         <v>41</v>
       </c>
       <c r="J216" t="b">
@@ -14095,7 +14065,7 @@
         <v>12</v>
       </c>
       <c r="B217" s="2" t="str">
-        <f>HYPERLINK(P217)</f>
+        <f t="shared" si="13"/>
         <v>https://iwp6.iwphys.org/animation/winters-ncssm-2009/torque-disc-01b.iwp</v>
       </c>
       <c r="D217" t="s">
@@ -14114,7 +14084,7 @@
         <v>6</v>
       </c>
       <c r="I217">
-        <f>H217/G217</f>
+        <f t="shared" si="15"/>
         <v>6</v>
       </c>
       <c r="J217" t="b">
@@ -14144,7 +14114,7 @@
         <v>12</v>
       </c>
       <c r="B218" s="2" t="str">
-        <f>HYPERLINK(P218)</f>
+        <f t="shared" si="13"/>
         <v>https://iwp6.iwphys.org/animation/winters-ncssm-2009/torque-disc-02.iwp</v>
       </c>
       <c r="D218" t="s">
@@ -14163,7 +14133,7 @@
         <v>4</v>
       </c>
       <c r="I218">
-        <f>H218/G218</f>
+        <f t="shared" si="15"/>
         <v>4</v>
       </c>
       <c r="J218" t="b">
@@ -14193,7 +14163,7 @@
         <v>12</v>
       </c>
       <c r="B219" s="2" t="str">
-        <f>HYPERLINK(P219)</f>
+        <f t="shared" si="13"/>
         <v>https://iwp6.iwphys.org/animation/winters-ncssm-2009/torque-disc-03.iwp</v>
       </c>
       <c r="D219" t="s">
@@ -14212,7 +14182,7 @@
         <v>5</v>
       </c>
       <c r="I219">
-        <f>H219/G219</f>
+        <f t="shared" si="15"/>
         <v>5</v>
       </c>
       <c r="J219" t="b">
@@ -14242,7 +14212,7 @@
         <v>12</v>
       </c>
       <c r="B220" s="2" t="str">
-        <f>HYPERLINK(P220)</f>
+        <f t="shared" si="13"/>
         <v>https://iwp6.iwphys.org/animation/winters-ncssm-2009/trav-wave-2.iwp</v>
       </c>
       <c r="D220" t="s">
@@ -14261,7 +14231,7 @@
         <v>13</v>
       </c>
       <c r="I220">
-        <f>H220/G220</f>
+        <f t="shared" si="15"/>
         <v>13</v>
       </c>
       <c r="J220" t="b">
@@ -14291,7 +14261,7 @@
         <v>12</v>
       </c>
       <c r="B221" s="2" t="str">
-        <f>HYPERLINK(P221)</f>
+        <f t="shared" si="13"/>
         <v>https://iwp6.iwphys.org/animation/winters-ncssm-2009/trav-wave-3.iwp</v>
       </c>
       <c r="D221" t="s">
@@ -14310,7 +14280,7 @@
         <v>23</v>
       </c>
       <c r="I221">
-        <f>H221/G221</f>
+        <f t="shared" si="15"/>
         <v>23</v>
       </c>
       <c r="J221" t="b">
@@ -14340,7 +14310,7 @@
         <v>12</v>
       </c>
       <c r="B222" s="2" t="str">
-        <f>HYPERLINK(P222)</f>
+        <f t="shared" si="13"/>
         <v>https://iwp6.iwphys.org/animation/winters-ncssm-2009/vector02.iwp</v>
       </c>
       <c r="D222" t="s">
@@ -14388,7 +14358,7 @@
         <v>12</v>
       </c>
       <c r="B223" s="2" t="str">
-        <f>HYPERLINK(P223)</f>
+        <f t="shared" si="13"/>
         <v>https://iwp6.iwphys.org/animation/winters-ncssm-2009/vector03.iwp</v>
       </c>
       <c r="D223" t="s">
@@ -14436,7 +14406,7 @@
         <v>12</v>
       </c>
       <c r="B224" s="2" t="str">
-        <f>HYPERLINK(P224)</f>
+        <f t="shared" si="13"/>
         <v>https://iwp6.iwphys.org/animation/winters-ncssm-2009/velocity01b.iwp</v>
       </c>
       <c r="D224" t="s">
@@ -14485,7 +14455,7 @@
         <v>12</v>
       </c>
       <c r="B225" s="2" t="str">
-        <f>HYPERLINK(P225)</f>
+        <f t="shared" si="13"/>
         <v>https://iwp6.iwphys.org/animation/winters-ncssm-2009/vertical-spring-analysis-2.iwp</v>
       </c>
       <c r="D225" t="s">
@@ -14534,7 +14504,7 @@
         <v>12</v>
       </c>
       <c r="B226" s="2" t="str">
-        <f>HYPERLINK(P226)</f>
+        <f t="shared" si="13"/>
         <v>https://iwp6.iwphys.org/animation/winters-ncssm-2009/vertical-spring-analysis-3.iwp</v>
       </c>
       <c r="D226" t="s">
@@ -14583,7 +14553,7 @@
         <v>12</v>
       </c>
       <c r="B227" s="2" t="str">
-        <f>HYPERLINK(P227)</f>
+        <f t="shared" si="13"/>
         <v>https://iwp6.iwphys.org/animation/winters-ncssm-2009/window01.iwp</v>
       </c>
       <c r="D227" t="s">

</xml_diff>